<commit_message>
Aggiunta lettura lista slides da generare
</commit_message>
<xml_diff>
--- a/Solution/FilesEditor.Tests/TestFiles/Templates/DataSource_Template.xlsx
+++ b/Solution/FilesEditor.Tests/TestFiles/Templates/DataSource_Template.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\Lefo\Dev\3 GDPptGenerator\Solution\PptGeneratorGUI\Configurazione\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\Lefo\Dev\3 GDPptGenerator\Solution\FilesEditor.Tests\TestFiles\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="16215" tabRatio="851" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="16215" tabRatio="851" firstSheet="5" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="Superdettagli" sheetId="1" r:id="rId1"/>
@@ -28,9 +28,12 @@
     <sheet name="PP_09" sheetId="14" r:id="rId14"/>
     <sheet name="PP_10" sheetId="15" r:id="rId15"/>
     <sheet name="PP_11" sheetId="16" r:id="rId16"/>
+    <sheet name="PP_12" sheetId="17" r:id="rId17"/>
   </sheets>
   <definedNames>
+    <definedName name="tblFieldFilters" localSheetId="16">Table9[]</definedName>
     <definedName name="tblFieldFilters">Table9[]</definedName>
+    <definedName name="tblIndexPowerpoint" localSheetId="16">Table8[]</definedName>
     <definedName name="tblIndexPowerpoint">Table8[]</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
@@ -54,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="237">
   <si>
     <t>da considerare?_</t>
   </si>
@@ -681,15 +684,6 @@
   </si>
   <si>
     <t>PP_11</t>
-  </si>
-  <si>
-    <t>PP_12</t>
-  </si>
-  <si>
-    <t>PP_13</t>
-  </si>
-  <si>
-    <t>PP_14</t>
   </si>
   <si>
     <t>Engineering KPI_Sales.pptx</t>
@@ -793,13 +787,13 @@
     <t>Progetti D dettaglio</t>
   </si>
   <si>
-    <t>Progetti M</t>
-  </si>
-  <si>
     <t>Progetti U (improduttive)</t>
   </si>
   <si>
     <t>Progetti U (produttive indirette)</t>
+  </si>
+  <si>
+    <t>PP_12</t>
   </si>
 </sst>
 </file>
@@ -1087,7 +1081,7 @@
         <xdr:cNvPr id="2" name="Group 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{356DB1C8-B726-46E4-A37C-5DCDC3B56533}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{356DB1C8-B726-46E4-A37C-5DCDC3B56533}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1106,7 +1100,7 @@
           <xdr:cNvPr id="3" name="Rectangle 2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DD69F98F-C2DE-5B3D-AD9B-1385703EAAA4}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{DD69F98F-C2DE-5B3D-AD9B-1385703EAAA4}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1154,7 +1148,7 @@
           <xdr:cNvPr id="4" name="TextBox 3">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C8757078-1A93-B150-D490-CB5780B9E446}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C8757078-1A93-B150-D490-CB5780B9E446}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1202,7 +1196,7 @@
           <xdr:cNvPr id="5" name="TextBox 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{17B2414E-36D9-F9DA-F440-862ABDE6A5AB}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{17B2414E-36D9-F9DA-F440-862ABDE6A5AB}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1266,7 +1260,7 @@
         <xdr:cNvPr id="6" name="Straight Connector 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E3FA2292-5CF5-4E38-A2EA-A37A8220D345}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E3FA2292-5CF5-4E38-A2EA-A37A8220D345}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1324,7 +1318,7 @@
         <xdr:cNvPr id="7" name="Group 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A662FB5B-1B8C-482D-BB22-DD7634AD884E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A662FB5B-1B8C-482D-BB22-DD7634AD884E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1343,7 +1337,7 @@
           <xdr:cNvPr id="8" name="Rectangle 7">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{743BEFAD-47AE-F721-807C-ADED1AA08EF3}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{743BEFAD-47AE-F721-807C-ADED1AA08EF3}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1391,7 +1385,7 @@
           <xdr:cNvPr id="9" name="Straight Connector 8">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{23D0CA46-A1A1-244F-C51D-72BDB41B6C93}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{23D0CA46-A1A1-244F-C51D-72BDB41B6C93}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1434,7 +1428,7 @@
           <xdr:cNvPr id="10" name="TextBox 9">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C43F6D6B-ABEB-6881-ABD1-806AACA964EC}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C43F6D6B-ABEB-6881-ABD1-806AACA964EC}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1482,7 +1476,7 @@
           <xdr:cNvPr id="11" name="TextBox 10">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B98B25C0-EF27-4688-FA6A-E00624852F57}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B98B25C0-EF27-4688-FA6A-E00624852F57}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2812,7 +2806,7 @@
   <sheetData>
     <row r="1" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B1" s="17"/>
       <c r="C1" s="6"/>
@@ -2832,10 +2826,10 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="10"/>
@@ -3326,7 +3320,7 @@
   <sheetData>
     <row r="1" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B1" s="17"/>
       <c r="C1" s="6"/>
@@ -3346,10 +3340,10 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="10"/>
@@ -3840,7 +3834,7 @@
   <sheetData>
     <row r="1" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B1" s="17"/>
       <c r="C1" s="6"/>
@@ -3860,10 +3854,10 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="10"/>
@@ -4354,7 +4348,7 @@
   <sheetData>
     <row r="1" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B1" s="17"/>
       <c r="C1" s="6"/>
@@ -4374,10 +4368,10 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="10"/>
@@ -4868,7 +4862,7 @@
   <sheetData>
     <row r="1" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B1" s="17"/>
       <c r="C1" s="6"/>
@@ -4888,10 +4882,10 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="10"/>
@@ -5382,7 +5376,7 @@
   <sheetData>
     <row r="1" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B1" s="17"/>
       <c r="C1" s="6"/>
@@ -5402,10 +5396,10 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="10"/>
@@ -5896,7 +5890,7 @@
   <sheetData>
     <row r="1" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B1" s="17"/>
       <c r="C1" s="6"/>
@@ -5916,10 +5910,524 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>224</v>
+        <v>221</v>
+      </c>
+      <c r="C2" s="9"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="10"/>
+      <c r="N2" s="10"/>
+      <c r="O2" s="10"/>
+      <c r="P2" s="11"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="4"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="10"/>
+      <c r="O3" s="10"/>
+      <c r="P3" s="11"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C4" s="9"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="10"/>
+      <c r="O4" s="10"/>
+      <c r="P4" s="11"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C5" s="9"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
+      <c r="M5" s="10"/>
+      <c r="N5" s="10"/>
+      <c r="O5" s="10"/>
+      <c r="P5" s="11"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C6" s="9"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10"/>
+      <c r="M6" s="10"/>
+      <c r="N6" s="10"/>
+      <c r="O6" s="10"/>
+      <c r="P6" s="11"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C7" s="9"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="10"/>
+      <c r="N7" s="10"/>
+      <c r="O7" s="10"/>
+      <c r="P7" s="11"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C8" s="9"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="10"/>
+      <c r="N8" s="10"/>
+      <c r="O8" s="10"/>
+      <c r="P8" s="11"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C9" s="9"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="10"/>
+      <c r="N9" s="10"/>
+      <c r="O9" s="10"/>
+      <c r="P9" s="11"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C10" s="9"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="10"/>
+      <c r="N10" s="10"/>
+      <c r="O10" s="10"/>
+      <c r="P10" s="11"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C11" s="9"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="10"/>
+      <c r="N11" s="10"/>
+      <c r="O11" s="10"/>
+      <c r="P11" s="11"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C12" s="9"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="10"/>
+      <c r="M12" s="10"/>
+      <c r="N12" s="10"/>
+      <c r="O12" s="10"/>
+      <c r="P12" s="11"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C13" s="9"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="10"/>
+      <c r="N13" s="10"/>
+      <c r="O13" s="10"/>
+      <c r="P13" s="11"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C14" s="9"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="10"/>
+      <c r="N14" s="10"/>
+      <c r="O14" s="10"/>
+      <c r="P14" s="11"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C15" s="9"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="10"/>
+      <c r="M15" s="10"/>
+      <c r="N15" s="10"/>
+      <c r="O15" s="10"/>
+      <c r="P15" s="11"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C16" s="9"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="10"/>
+      <c r="M16" s="10"/>
+      <c r="N16" s="10"/>
+      <c r="O16" s="10"/>
+      <c r="P16" s="11"/>
+    </row>
+    <row r="17" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C17" s="9"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="10"/>
+      <c r="K17" s="10"/>
+      <c r="L17" s="10"/>
+      <c r="M17" s="10"/>
+      <c r="N17" s="10"/>
+      <c r="O17" s="10"/>
+      <c r="P17" s="11"/>
+    </row>
+    <row r="18" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C18" s="9"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="10"/>
+      <c r="K18" s="10"/>
+      <c r="L18" s="10"/>
+      <c r="M18" s="10"/>
+      <c r="N18" s="10"/>
+      <c r="O18" s="10"/>
+      <c r="P18" s="11"/>
+    </row>
+    <row r="19" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C19" s="9"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="10"/>
+      <c r="K19" s="10"/>
+      <c r="L19" s="10"/>
+      <c r="M19" s="10"/>
+      <c r="N19" s="10"/>
+      <c r="O19" s="10"/>
+      <c r="P19" s="11"/>
+    </row>
+    <row r="20" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C20" s="9"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="10"/>
+      <c r="K20" s="10"/>
+      <c r="L20" s="10"/>
+      <c r="M20" s="10"/>
+      <c r="N20" s="10"/>
+      <c r="O20" s="10"/>
+      <c r="P20" s="11"/>
+    </row>
+    <row r="21" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C21" s="9"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="10"/>
+      <c r="K21" s="10"/>
+      <c r="L21" s="10"/>
+      <c r="M21" s="10"/>
+      <c r="N21" s="10"/>
+      <c r="O21" s="10"/>
+      <c r="P21" s="11"/>
+    </row>
+    <row r="22" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C22" s="9"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="10"/>
+      <c r="J22" s="10"/>
+      <c r="K22" s="10"/>
+      <c r="L22" s="10"/>
+      <c r="M22" s="10"/>
+      <c r="N22" s="10"/>
+      <c r="O22" s="10"/>
+      <c r="P22" s="11"/>
+    </row>
+    <row r="23" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C23" s="9"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="10"/>
+      <c r="I23" s="10"/>
+      <c r="J23" s="10"/>
+      <c r="K23" s="10"/>
+      <c r="L23" s="10"/>
+      <c r="M23" s="10"/>
+      <c r="N23" s="10"/>
+      <c r="O23" s="10"/>
+      <c r="P23" s="11"/>
+    </row>
+    <row r="24" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C24" s="9"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="10"/>
+      <c r="I24" s="10"/>
+      <c r="J24" s="10"/>
+      <c r="K24" s="10"/>
+      <c r="L24" s="10"/>
+      <c r="M24" s="10"/>
+      <c r="N24" s="10"/>
+      <c r="O24" s="10"/>
+      <c r="P24" s="11"/>
+    </row>
+    <row r="25" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C25" s="9"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="10"/>
+      <c r="I25" s="10"/>
+      <c r="J25" s="10"/>
+      <c r="K25" s="10"/>
+      <c r="L25" s="10"/>
+      <c r="M25" s="10"/>
+      <c r="N25" s="10"/>
+      <c r="O25" s="10"/>
+      <c r="P25" s="11"/>
+    </row>
+    <row r="26" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C26" s="9"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="10"/>
+      <c r="I26" s="10"/>
+      <c r="J26" s="10"/>
+      <c r="K26" s="10"/>
+      <c r="L26" s="10"/>
+      <c r="M26" s="10"/>
+      <c r="N26" s="10"/>
+      <c r="O26" s="10"/>
+      <c r="P26" s="11"/>
+    </row>
+    <row r="27" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C27" s="9"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="10"/>
+      <c r="I27" s="10"/>
+      <c r="J27" s="10"/>
+      <c r="K27" s="10"/>
+      <c r="L27" s="10"/>
+      <c r="M27" s="10"/>
+      <c r="N27" s="10"/>
+      <c r="O27" s="10"/>
+      <c r="P27" s="11"/>
+    </row>
+    <row r="28" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C28" s="9"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="10"/>
+      <c r="H28" s="10"/>
+      <c r="I28" s="10"/>
+      <c r="J28" s="10"/>
+      <c r="K28" s="10"/>
+      <c r="L28" s="10"/>
+      <c r="M28" s="10"/>
+      <c r="N28" s="10"/>
+      <c r="O28" s="10"/>
+      <c r="P28" s="11"/>
+    </row>
+    <row r="29" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C29" s="9"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="10"/>
+      <c r="G29" s="10"/>
+      <c r="H29" s="10"/>
+      <c r="I29" s="10"/>
+      <c r="J29" s="10"/>
+      <c r="K29" s="10"/>
+      <c r="L29" s="10"/>
+      <c r="M29" s="10"/>
+      <c r="N29" s="10"/>
+      <c r="O29" s="10"/>
+      <c r="P29" s="11"/>
+    </row>
+    <row r="30" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C30" s="12"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="13"/>
+      <c r="H30" s="13"/>
+      <c r="I30" s="13"/>
+      <c r="J30" s="13"/>
+      <c r="K30" s="13"/>
+      <c r="L30" s="13"/>
+      <c r="M30" s="13"/>
+      <c r="N30" s="13"/>
+      <c r="O30" s="13"/>
+      <c r="P30" s="14"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
+        <v>220</v>
+      </c>
+      <c r="B1" s="17"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="8"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>221</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="10"/>
@@ -6892,7 +7400,7 @@
   <dimension ref="A1:Z93"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6910,7 +7418,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B1" s="15"/>
       <c r="C1" s="15"/>
@@ -6920,7 +7428,7 @@
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
       <c r="K1" s="16" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="L1" s="16"/>
     </row>
@@ -6941,7 +7449,7 @@
         <v>190</v>
       </c>
       <c r="B3" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="C3" t="s">
         <v>191</v>
@@ -6958,10 +7466,10 @@
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
       <c r="K3" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="L3" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -6969,7 +7477,7 @@
         <v>195</v>
       </c>
       <c r="B4" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>196</v>
@@ -6984,11 +7492,11 @@
         <v>199</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="I4" s="3"/>
       <c r="K4" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="L4" t="s">
         <v>7</v>
@@ -6999,7 +7507,7 @@
         <v>195</v>
       </c>
       <c r="B5" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>197</v>
@@ -7009,7 +7517,7 @@
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
       <c r="K5" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="L5" t="s">
         <v>8</v>
@@ -7020,7 +7528,7 @@
         <v>195</v>
       </c>
       <c r="B6" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>200</v>
@@ -7030,7 +7538,7 @@
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
       <c r="K6" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="L6" t="s">
         <v>156</v>
@@ -7041,7 +7549,7 @@
         <v>195</v>
       </c>
       <c r="B7" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>201</v>
@@ -7051,7 +7559,7 @@
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
       <c r="K7" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="L7" t="s">
         <v>157</v>
@@ -7062,7 +7570,7 @@
         <v>195</v>
       </c>
       <c r="B8" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>202</v>
@@ -7072,7 +7580,7 @@
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
       <c r="K8" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="L8" t="s">
         <v>128</v>
@@ -7083,7 +7591,7 @@
         <v>195</v>
       </c>
       <c r="B9" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>198</v>
@@ -7098,7 +7606,7 @@
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
       <c r="K9" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="L9" t="s">
         <v>4</v>
@@ -7109,7 +7617,7 @@
         <v>195</v>
       </c>
       <c r="B10" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>203</v>
@@ -7117,11 +7625,11 @@
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="H10" s="3" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="I10" s="3"/>
       <c r="K10" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="L10" t="s">
         <v>24</v>
@@ -7132,17 +7640,24 @@
         <v>195</v>
       </c>
       <c r="B11" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
+      <c r="D11" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="F11" t="s">
+        <v>199</v>
+      </c>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
       <c r="K11" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="L11" t="s">
         <v>158</v>
@@ -7153,7 +7668,7 @@
         <v>195</v>
       </c>
       <c r="B12" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>207</v>
@@ -7170,7 +7685,7 @@
         <v>195</v>
       </c>
       <c r="B13" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>205</v>
@@ -7187,7 +7702,7 @@
         <v>195</v>
       </c>
       <c r="B14" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>208</v>
@@ -7201,15 +7716,17 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>195</v>
+        <v>209</v>
       </c>
       <c r="B15" t="s">
-        <v>237</v>
+        <v>223</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="D15" s="1"/>
+        <v>196</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>201</v>
+      </c>
       <c r="E15" s="1"/>
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
@@ -7218,13 +7735,13 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>195</v>
+        <v>209</v>
       </c>
       <c r="B16" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -7235,23 +7752,16 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>195</v>
+        <v>209</v>
       </c>
       <c r="B17" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="F17" t="s">
-        <v>199</v>
-      </c>
+        <v>236</v>
+      </c>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
       <c r="K17" s="3"/>
@@ -7259,16 +7769,23 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B18" t="s">
         <v>226</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
+        <v>201</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="F18" t="s">
+        <v>199</v>
+      </c>
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
       <c r="K18" s="3"/>
@@ -7276,16 +7793,14 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B19" t="s">
-        <v>238</v>
+        <v>227</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
+        <v>202</v>
+      </c>
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
       <c r="K19" s="3"/>
@@ -7293,16 +7808,14 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B20" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
+        <v>208</v>
+      </c>
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
       <c r="K20" s="3"/>
@@ -7310,61 +7823,39 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B21" t="s">
         <v>229</v>
       </c>
       <c r="C21" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
       <c r="K21" s="3"/>
       <c r="L21" s="3"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>212</v>
-      </c>
-      <c r="B22" t="s">
-        <v>230</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>202</v>
-      </c>
+      <c r="C22" s="1"/>
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
       <c r="K22" s="3"/>
       <c r="L22" s="3"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>212</v>
-      </c>
-      <c r="B23" t="s">
-        <v>236</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>208</v>
-      </c>
+      <c r="C23" s="1"/>
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
       <c r="K23" s="3"/>
       <c r="L23" s="3"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>212</v>
-      </c>
-      <c r="B24" t="s">
-        <v>232</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>203</v>
-      </c>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
       <c r="H24" s="3"/>
       <c r="I24" s="3"/>
       <c r="K24" s="3"/>
@@ -7817,7 +8308,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
@@ -7829,7 +8320,7 @@
   <sheetData>
     <row r="1" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B1" s="17"/>
       <c r="C1" s="6"/>
@@ -7850,10 +8341,10 @@
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="10"/>
@@ -8390,7 +8881,7 @@
   <sheetData>
     <row r="1" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B1" s="17"/>
       <c r="C1" s="6"/>
@@ -8410,10 +8901,10 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="10"/>
@@ -8904,7 +9395,7 @@
   <sheetData>
     <row r="1" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B1" s="17"/>
       <c r="C1" s="6"/>
@@ -8924,10 +9415,10 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="10"/>
@@ -9418,7 +9909,7 @@
   <sheetData>
     <row r="1" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B1" s="17"/>
       <c r="C1" s="6"/>
@@ -9438,10 +9929,10 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="10"/>

</xml_diff>

<commit_message>
Aggiunte opzioni Append data e corretto Ran Rate in Run Rate
</commit_message>
<xml_diff>
--- a/Solution/FilesEditor.Tests/TestFiles/Templates/DataSource_Template.xlsx
+++ b/Solution/FilesEditor.Tests/TestFiles/Templates/DataSource_Template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="16215" tabRatio="851" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="16220" tabRatio="851" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Superdettagli" sheetId="1" r:id="rId1"/>
@@ -1089,8 +1089,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="8296334" y="800101"/>
-          <a:ext cx="1154801" cy="713013"/>
+          <a:off x="8696660" y="766971"/>
+          <a:ext cx="1149280" cy="688165"/>
           <a:chOff x="1230086" y="4294415"/>
           <a:chExt cx="1151488" cy="713013"/>
         </a:xfrm>
@@ -1326,8 +1326,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="8318110" y="1948543"/>
-          <a:ext cx="1129985" cy="745671"/>
+          <a:off x="8718436" y="1865717"/>
+          <a:ext cx="1124464" cy="712540"/>
           <a:chOff x="1230090" y="5464629"/>
           <a:chExt cx="1126672" cy="745671"/>
         </a:xfrm>
@@ -2014,66 +2014,66 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.140625" customWidth="1"/>
-    <col min="3" max="3" width="50.42578125" customWidth="1"/>
+    <col min="1" max="1" width="18.1796875" customWidth="1"/>
+    <col min="3" max="3" width="50.453125" customWidth="1"/>
     <col min="5" max="5" width="12" customWidth="1"/>
-    <col min="6" max="6" width="13.85546875" customWidth="1"/>
-    <col min="7" max="8" width="20.140625" customWidth="1"/>
+    <col min="6" max="6" width="13.81640625" customWidth="1"/>
+    <col min="7" max="8" width="20.1796875" customWidth="1"/>
     <col min="9" max="9" width="25" customWidth="1"/>
     <col min="23" max="23" width="14" customWidth="1"/>
-    <col min="24" max="24" width="12.7109375" customWidth="1"/>
-    <col min="25" max="25" width="23.28515625" customWidth="1"/>
-    <col min="26" max="27" width="18.7109375" customWidth="1"/>
-    <col min="28" max="28" width="20.42578125" customWidth="1"/>
+    <col min="24" max="24" width="12.7265625" customWidth="1"/>
+    <col min="25" max="25" width="23.26953125" customWidth="1"/>
+    <col min="26" max="27" width="18.7265625" customWidth="1"/>
+    <col min="28" max="28" width="20.453125" customWidth="1"/>
     <col min="29" max="29" width="21" customWidth="1"/>
-    <col min="30" max="30" width="17.140625" customWidth="1"/>
-    <col min="32" max="32" width="20.140625" customWidth="1"/>
-    <col min="33" max="33" width="21.7109375" customWidth="1"/>
-    <col min="34" max="34" width="19.85546875" customWidth="1"/>
+    <col min="30" max="30" width="17.1796875" customWidth="1"/>
+    <col min="32" max="32" width="20.1796875" customWidth="1"/>
+    <col min="33" max="33" width="21.7265625" customWidth="1"/>
+    <col min="34" max="34" width="19.81640625" customWidth="1"/>
     <col min="35" max="35" width="20" customWidth="1"/>
-    <col min="36" max="36" width="15.140625" customWidth="1"/>
-    <col min="37" max="37" width="10.85546875" customWidth="1"/>
-    <col min="38" max="38" width="19.7109375" customWidth="1"/>
-    <col min="39" max="39" width="16.85546875" customWidth="1"/>
-    <col min="40" max="40" width="12.85546875" customWidth="1"/>
-    <col min="41" max="41" width="13.42578125" customWidth="1"/>
-    <col min="42" max="42" width="22.42578125" customWidth="1"/>
-    <col min="43" max="43" width="11.7109375" customWidth="1"/>
-    <col min="44" max="44" width="10.42578125" customWidth="1"/>
-    <col min="45" max="45" width="11.7109375" customWidth="1"/>
-    <col min="46" max="46" width="10.140625" customWidth="1"/>
+    <col min="36" max="36" width="15.1796875" customWidth="1"/>
+    <col min="37" max="37" width="10.81640625" customWidth="1"/>
+    <col min="38" max="38" width="19.7265625" customWidth="1"/>
+    <col min="39" max="39" width="16.81640625" customWidth="1"/>
+    <col min="40" max="40" width="12.81640625" customWidth="1"/>
+    <col min="41" max="41" width="13.453125" customWidth="1"/>
+    <col min="42" max="42" width="22.453125" customWidth="1"/>
+    <col min="43" max="43" width="11.7265625" customWidth="1"/>
+    <col min="44" max="44" width="10.453125" customWidth="1"/>
+    <col min="45" max="45" width="11.7265625" customWidth="1"/>
+    <col min="46" max="46" width="10.1796875" customWidth="1"/>
     <col min="47" max="47" width="11" customWidth="1"/>
-    <col min="48" max="48" width="20.5703125" customWidth="1"/>
-    <col min="49" max="49" width="12.85546875" customWidth="1"/>
-    <col min="50" max="50" width="14.85546875" customWidth="1"/>
-    <col min="51" max="51" width="12.140625" customWidth="1"/>
-    <col min="52" max="52" width="15.42578125" customWidth="1"/>
-    <col min="53" max="53" width="14.28515625" customWidth="1"/>
+    <col min="48" max="48" width="20.54296875" customWidth="1"/>
+    <col min="49" max="49" width="12.81640625" customWidth="1"/>
+    <col min="50" max="50" width="14.81640625" customWidth="1"/>
+    <col min="51" max="51" width="12.1796875" customWidth="1"/>
+    <col min="52" max="52" width="15.453125" customWidth="1"/>
+    <col min="53" max="53" width="14.26953125" customWidth="1"/>
     <col min="54" max="54" width="19" customWidth="1"/>
-    <col min="55" max="55" width="11.5703125" customWidth="1"/>
-    <col min="69" max="69" width="11.28515625" customWidth="1"/>
-    <col min="70" max="70" width="17.85546875" customWidth="1"/>
-    <col min="72" max="72" width="12.7109375" customWidth="1"/>
-    <col min="73" max="73" width="15.85546875" customWidth="1"/>
-    <col min="74" max="74" width="11.85546875" customWidth="1"/>
-    <col min="75" max="75" width="18.28515625" customWidth="1"/>
-    <col min="76" max="76" width="20.140625" customWidth="1"/>
-    <col min="77" max="77" width="45.7109375" customWidth="1"/>
-    <col min="78" max="78" width="16.5703125" customWidth="1"/>
-    <col min="79" max="79" width="25.7109375" customWidth="1"/>
-    <col min="80" max="80" width="27.140625" customWidth="1"/>
+    <col min="55" max="55" width="11.54296875" customWidth="1"/>
+    <col min="69" max="69" width="11.26953125" customWidth="1"/>
+    <col min="70" max="70" width="17.81640625" customWidth="1"/>
+    <col min="72" max="72" width="12.7265625" customWidth="1"/>
+    <col min="73" max="73" width="15.81640625" customWidth="1"/>
+    <col min="74" max="74" width="11.81640625" customWidth="1"/>
+    <col min="75" max="75" width="18.26953125" customWidth="1"/>
+    <col min="76" max="76" width="20.1796875" customWidth="1"/>
+    <col min="77" max="77" width="45.7265625" customWidth="1"/>
+    <col min="78" max="78" width="16.54296875" customWidth="1"/>
+    <col min="79" max="79" width="25.7265625" customWidth="1"/>
+    <col min="80" max="80" width="27.1796875" customWidth="1"/>
     <col min="81" max="81" width="17" customWidth="1"/>
-    <col min="82" max="82" width="19.140625" customWidth="1"/>
-    <col min="83" max="83" width="15.28515625" customWidth="1"/>
-    <col min="84" max="85" width="10.85546875" customWidth="1"/>
-    <col min="86" max="86" width="10.28515625" customWidth="1"/>
-    <col min="87" max="87" width="15.140625" customWidth="1"/>
-    <col min="90" max="90" width="21.5703125" customWidth="1"/>
+    <col min="82" max="82" width="19.1796875" customWidth="1"/>
+    <col min="83" max="83" width="15.26953125" customWidth="1"/>
+    <col min="84" max="85" width="10.81640625" customWidth="1"/>
+    <col min="86" max="86" width="10.26953125" customWidth="1"/>
+    <col min="87" max="87" width="15.1796875" customWidth="1"/>
+    <col min="90" max="90" width="21.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:90" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:90" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2345,7 +2345,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:90" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:90" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>90</v>
       </c>
@@ -2563,7 +2563,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="3" spans="1:90" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:90" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>90</v>
       </c>
@@ -2798,13 +2798,13 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" customWidth="1"/>
-    <col min="2" max="2" width="25.7109375" customWidth="1"/>
+    <col min="1" max="1" width="10.7265625" customWidth="1"/>
+    <col min="2" max="2" width="25.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="17" t="s">
         <v>220</v>
       </c>
@@ -2824,7 +2824,7 @@
       <c r="O1" s="7"/>
       <c r="P1" s="8"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>219</v>
       </c>
@@ -2846,7 +2846,7 @@
       <c r="O2" s="10"/>
       <c r="P2" s="11"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3" s="4"/>
       <c r="B3" s="5"/>
       <c r="C3" s="9"/>
@@ -2864,7 +2864,7 @@
       <c r="O3" s="10"/>
       <c r="P3" s="11"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C4" s="9"/>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -2880,7 +2880,7 @@
       <c r="O4" s="10"/>
       <c r="P4" s="11"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C5" s="9"/>
       <c r="D5" s="10"/>
       <c r="E5" s="10"/>
@@ -2896,7 +2896,7 @@
       <c r="O5" s="10"/>
       <c r="P5" s="11"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C6" s="9"/>
       <c r="D6" s="10"/>
       <c r="E6" s="10"/>
@@ -2912,7 +2912,7 @@
       <c r="O6" s="10"/>
       <c r="P6" s="11"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C7" s="9"/>
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
@@ -2928,7 +2928,7 @@
       <c r="O7" s="10"/>
       <c r="P7" s="11"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C8" s="9"/>
       <c r="D8" s="10"/>
       <c r="E8" s="10"/>
@@ -2944,7 +2944,7 @@
       <c r="O8" s="10"/>
       <c r="P8" s="11"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C9" s="9"/>
       <c r="D9" s="10"/>
       <c r="E9" s="10"/>
@@ -2960,7 +2960,7 @@
       <c r="O9" s="10"/>
       <c r="P9" s="11"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C10" s="9"/>
       <c r="D10" s="10"/>
       <c r="E10" s="10"/>
@@ -2976,7 +2976,7 @@
       <c r="O10" s="10"/>
       <c r="P10" s="11"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C11" s="9"/>
       <c r="D11" s="10"/>
       <c r="E11" s="10"/>
@@ -2992,7 +2992,7 @@
       <c r="O11" s="10"/>
       <c r="P11" s="11"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C12" s="9"/>
       <c r="D12" s="10"/>
       <c r="E12" s="10"/>
@@ -3008,7 +3008,7 @@
       <c r="O12" s="10"/>
       <c r="P12" s="11"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C13" s="9"/>
       <c r="D13" s="10"/>
       <c r="E13" s="10"/>
@@ -3024,7 +3024,7 @@
       <c r="O13" s="10"/>
       <c r="P13" s="11"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C14" s="9"/>
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
@@ -3040,7 +3040,7 @@
       <c r="O14" s="10"/>
       <c r="P14" s="11"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C15" s="9"/>
       <c r="D15" s="10"/>
       <c r="E15" s="10"/>
@@ -3056,7 +3056,7 @@
       <c r="O15" s="10"/>
       <c r="P15" s="11"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C16" s="9"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
@@ -3072,7 +3072,7 @@
       <c r="O16" s="10"/>
       <c r="P16" s="11"/>
     </row>
-    <row r="17" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C17" s="9"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
@@ -3088,7 +3088,7 @@
       <c r="O17" s="10"/>
       <c r="P17" s="11"/>
     </row>
-    <row r="18" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C18" s="9"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
@@ -3104,7 +3104,7 @@
       <c r="O18" s="10"/>
       <c r="P18" s="11"/>
     </row>
-    <row r="19" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C19" s="9"/>
       <c r="D19" s="10"/>
       <c r="E19" s="10"/>
@@ -3120,7 +3120,7 @@
       <c r="O19" s="10"/>
       <c r="P19" s="11"/>
     </row>
-    <row r="20" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C20" s="9"/>
       <c r="D20" s="10"/>
       <c r="E20" s="10"/>
@@ -3136,7 +3136,7 @@
       <c r="O20" s="10"/>
       <c r="P20" s="11"/>
     </row>
-    <row r="21" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C21" s="9"/>
       <c r="D21" s="10"/>
       <c r="E21" s="10"/>
@@ -3152,7 +3152,7 @@
       <c r="O21" s="10"/>
       <c r="P21" s="11"/>
     </row>
-    <row r="22" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C22" s="9"/>
       <c r="D22" s="10"/>
       <c r="E22" s="10"/>
@@ -3168,7 +3168,7 @@
       <c r="O22" s="10"/>
       <c r="P22" s="11"/>
     </row>
-    <row r="23" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C23" s="9"/>
       <c r="D23" s="10"/>
       <c r="E23" s="10"/>
@@ -3184,7 +3184,7 @@
       <c r="O23" s="10"/>
       <c r="P23" s="11"/>
     </row>
-    <row r="24" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C24" s="9"/>
       <c r="D24" s="10"/>
       <c r="E24" s="10"/>
@@ -3200,7 +3200,7 @@
       <c r="O24" s="10"/>
       <c r="P24" s="11"/>
     </row>
-    <row r="25" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C25" s="9"/>
       <c r="D25" s="10"/>
       <c r="E25" s="10"/>
@@ -3216,7 +3216,7 @@
       <c r="O25" s="10"/>
       <c r="P25" s="11"/>
     </row>
-    <row r="26" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C26" s="9"/>
       <c r="D26" s="10"/>
       <c r="E26" s="10"/>
@@ -3232,7 +3232,7 @@
       <c r="O26" s="10"/>
       <c r="P26" s="11"/>
     </row>
-    <row r="27" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C27" s="9"/>
       <c r="D27" s="10"/>
       <c r="E27" s="10"/>
@@ -3248,7 +3248,7 @@
       <c r="O27" s="10"/>
       <c r="P27" s="11"/>
     </row>
-    <row r="28" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C28" s="9"/>
       <c r="D28" s="10"/>
       <c r="E28" s="10"/>
@@ -3264,7 +3264,7 @@
       <c r="O28" s="10"/>
       <c r="P28" s="11"/>
     </row>
-    <row r="29" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C29" s="9"/>
       <c r="D29" s="10"/>
       <c r="E29" s="10"/>
@@ -3280,7 +3280,7 @@
       <c r="O29" s="10"/>
       <c r="P29" s="11"/>
     </row>
-    <row r="30" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="3:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C30" s="12"/>
       <c r="D30" s="13"/>
       <c r="E30" s="13"/>
@@ -3312,13 +3312,13 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" customWidth="1"/>
-    <col min="2" max="2" width="25.7109375" customWidth="1"/>
+    <col min="1" max="1" width="10.7265625" customWidth="1"/>
+    <col min="2" max="2" width="25.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="17" t="s">
         <v>220</v>
       </c>
@@ -3338,7 +3338,7 @@
       <c r="O1" s="7"/>
       <c r="P1" s="8"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>219</v>
       </c>
@@ -3360,7 +3360,7 @@
       <c r="O2" s="10"/>
       <c r="P2" s="11"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3" s="4"/>
       <c r="B3" s="5"/>
       <c r="C3" s="9"/>
@@ -3378,7 +3378,7 @@
       <c r="O3" s="10"/>
       <c r="P3" s="11"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C4" s="9"/>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -3394,7 +3394,7 @@
       <c r="O4" s="10"/>
       <c r="P4" s="11"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C5" s="9"/>
       <c r="D5" s="10"/>
       <c r="E5" s="10"/>
@@ -3410,7 +3410,7 @@
       <c r="O5" s="10"/>
       <c r="P5" s="11"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C6" s="9"/>
       <c r="D6" s="10"/>
       <c r="E6" s="10"/>
@@ -3426,7 +3426,7 @@
       <c r="O6" s="10"/>
       <c r="P6" s="11"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C7" s="9"/>
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
@@ -3442,7 +3442,7 @@
       <c r="O7" s="10"/>
       <c r="P7" s="11"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C8" s="9"/>
       <c r="D8" s="10"/>
       <c r="E8" s="10"/>
@@ -3458,7 +3458,7 @@
       <c r="O8" s="10"/>
       <c r="P8" s="11"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C9" s="9"/>
       <c r="D9" s="10"/>
       <c r="E9" s="10"/>
@@ -3474,7 +3474,7 @@
       <c r="O9" s="10"/>
       <c r="P9" s="11"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C10" s="9"/>
       <c r="D10" s="10"/>
       <c r="E10" s="10"/>
@@ -3490,7 +3490,7 @@
       <c r="O10" s="10"/>
       <c r="P10" s="11"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C11" s="9"/>
       <c r="D11" s="10"/>
       <c r="E11" s="10"/>
@@ -3506,7 +3506,7 @@
       <c r="O11" s="10"/>
       <c r="P11" s="11"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C12" s="9"/>
       <c r="D12" s="10"/>
       <c r="E12" s="10"/>
@@ -3522,7 +3522,7 @@
       <c r="O12" s="10"/>
       <c r="P12" s="11"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C13" s="9"/>
       <c r="D13" s="10"/>
       <c r="E13" s="10"/>
@@ -3538,7 +3538,7 @@
       <c r="O13" s="10"/>
       <c r="P13" s="11"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C14" s="9"/>
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
@@ -3554,7 +3554,7 @@
       <c r="O14" s="10"/>
       <c r="P14" s="11"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C15" s="9"/>
       <c r="D15" s="10"/>
       <c r="E15" s="10"/>
@@ -3570,7 +3570,7 @@
       <c r="O15" s="10"/>
       <c r="P15" s="11"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C16" s="9"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
@@ -3586,7 +3586,7 @@
       <c r="O16" s="10"/>
       <c r="P16" s="11"/>
     </row>
-    <row r="17" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C17" s="9"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
@@ -3602,7 +3602,7 @@
       <c r="O17" s="10"/>
       <c r="P17" s="11"/>
     </row>
-    <row r="18" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C18" s="9"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
@@ -3618,7 +3618,7 @@
       <c r="O18" s="10"/>
       <c r="P18" s="11"/>
     </row>
-    <row r="19" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C19" s="9"/>
       <c r="D19" s="10"/>
       <c r="E19" s="10"/>
@@ -3634,7 +3634,7 @@
       <c r="O19" s="10"/>
       <c r="P19" s="11"/>
     </row>
-    <row r="20" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C20" s="9"/>
       <c r="D20" s="10"/>
       <c r="E20" s="10"/>
@@ -3650,7 +3650,7 @@
       <c r="O20" s="10"/>
       <c r="P20" s="11"/>
     </row>
-    <row r="21" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C21" s="9"/>
       <c r="D21" s="10"/>
       <c r="E21" s="10"/>
@@ -3666,7 +3666,7 @@
       <c r="O21" s="10"/>
       <c r="P21" s="11"/>
     </row>
-    <row r="22" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C22" s="9"/>
       <c r="D22" s="10"/>
       <c r="E22" s="10"/>
@@ -3682,7 +3682,7 @@
       <c r="O22" s="10"/>
       <c r="P22" s="11"/>
     </row>
-    <row r="23" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C23" s="9"/>
       <c r="D23" s="10"/>
       <c r="E23" s="10"/>
@@ -3698,7 +3698,7 @@
       <c r="O23" s="10"/>
       <c r="P23" s="11"/>
     </row>
-    <row r="24" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C24" s="9"/>
       <c r="D24" s="10"/>
       <c r="E24" s="10"/>
@@ -3714,7 +3714,7 @@
       <c r="O24" s="10"/>
       <c r="P24" s="11"/>
     </row>
-    <row r="25" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C25" s="9"/>
       <c r="D25" s="10"/>
       <c r="E25" s="10"/>
@@ -3730,7 +3730,7 @@
       <c r="O25" s="10"/>
       <c r="P25" s="11"/>
     </row>
-    <row r="26" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C26" s="9"/>
       <c r="D26" s="10"/>
       <c r="E26" s="10"/>
@@ -3746,7 +3746,7 @@
       <c r="O26" s="10"/>
       <c r="P26" s="11"/>
     </row>
-    <row r="27" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C27" s="9"/>
       <c r="D27" s="10"/>
       <c r="E27" s="10"/>
@@ -3762,7 +3762,7 @@
       <c r="O27" s="10"/>
       <c r="P27" s="11"/>
     </row>
-    <row r="28" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C28" s="9"/>
       <c r="D28" s="10"/>
       <c r="E28" s="10"/>
@@ -3778,7 +3778,7 @@
       <c r="O28" s="10"/>
       <c r="P28" s="11"/>
     </row>
-    <row r="29" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C29" s="9"/>
       <c r="D29" s="10"/>
       <c r="E29" s="10"/>
@@ -3794,7 +3794,7 @@
       <c r="O29" s="10"/>
       <c r="P29" s="11"/>
     </row>
-    <row r="30" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="3:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C30" s="12"/>
       <c r="D30" s="13"/>
       <c r="E30" s="13"/>
@@ -3826,13 +3826,13 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" customWidth="1"/>
-    <col min="2" max="2" width="25.7109375" customWidth="1"/>
+    <col min="1" max="1" width="10.7265625" customWidth="1"/>
+    <col min="2" max="2" width="25.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="17" t="s">
         <v>220</v>
       </c>
@@ -3852,7 +3852,7 @@
       <c r="O1" s="7"/>
       <c r="P1" s="8"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>219</v>
       </c>
@@ -3874,7 +3874,7 @@
       <c r="O2" s="10"/>
       <c r="P2" s="11"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3" s="4"/>
       <c r="B3" s="5"/>
       <c r="C3" s="9"/>
@@ -3892,7 +3892,7 @@
       <c r="O3" s="10"/>
       <c r="P3" s="11"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C4" s="9"/>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -3908,7 +3908,7 @@
       <c r="O4" s="10"/>
       <c r="P4" s="11"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C5" s="9"/>
       <c r="D5" s="10"/>
       <c r="E5" s="10"/>
@@ -3924,7 +3924,7 @@
       <c r="O5" s="10"/>
       <c r="P5" s="11"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C6" s="9"/>
       <c r="D6" s="10"/>
       <c r="E6" s="10"/>
@@ -3940,7 +3940,7 @@
       <c r="O6" s="10"/>
       <c r="P6" s="11"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C7" s="9"/>
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
@@ -3956,7 +3956,7 @@
       <c r="O7" s="10"/>
       <c r="P7" s="11"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C8" s="9"/>
       <c r="D8" s="10"/>
       <c r="E8" s="10"/>
@@ -3972,7 +3972,7 @@
       <c r="O8" s="10"/>
       <c r="P8" s="11"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C9" s="9"/>
       <c r="D9" s="10"/>
       <c r="E9" s="10"/>
@@ -3988,7 +3988,7 @@
       <c r="O9" s="10"/>
       <c r="P9" s="11"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C10" s="9"/>
       <c r="D10" s="10"/>
       <c r="E10" s="10"/>
@@ -4004,7 +4004,7 @@
       <c r="O10" s="10"/>
       <c r="P10" s="11"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C11" s="9"/>
       <c r="D11" s="10"/>
       <c r="E11" s="10"/>
@@ -4020,7 +4020,7 @@
       <c r="O11" s="10"/>
       <c r="P11" s="11"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C12" s="9"/>
       <c r="D12" s="10"/>
       <c r="E12" s="10"/>
@@ -4036,7 +4036,7 @@
       <c r="O12" s="10"/>
       <c r="P12" s="11"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C13" s="9"/>
       <c r="D13" s="10"/>
       <c r="E13" s="10"/>
@@ -4052,7 +4052,7 @@
       <c r="O13" s="10"/>
       <c r="P13" s="11"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C14" s="9"/>
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
@@ -4068,7 +4068,7 @@
       <c r="O14" s="10"/>
       <c r="P14" s="11"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C15" s="9"/>
       <c r="D15" s="10"/>
       <c r="E15" s="10"/>
@@ -4084,7 +4084,7 @@
       <c r="O15" s="10"/>
       <c r="P15" s="11"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C16" s="9"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
@@ -4100,7 +4100,7 @@
       <c r="O16" s="10"/>
       <c r="P16" s="11"/>
     </row>
-    <row r="17" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C17" s="9"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
@@ -4116,7 +4116,7 @@
       <c r="O17" s="10"/>
       <c r="P17" s="11"/>
     </row>
-    <row r="18" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C18" s="9"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
@@ -4132,7 +4132,7 @@
       <c r="O18" s="10"/>
       <c r="P18" s="11"/>
     </row>
-    <row r="19" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C19" s="9"/>
       <c r="D19" s="10"/>
       <c r="E19" s="10"/>
@@ -4148,7 +4148,7 @@
       <c r="O19" s="10"/>
       <c r="P19" s="11"/>
     </row>
-    <row r="20" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C20" s="9"/>
       <c r="D20" s="10"/>
       <c r="E20" s="10"/>
@@ -4164,7 +4164,7 @@
       <c r="O20" s="10"/>
       <c r="P20" s="11"/>
     </row>
-    <row r="21" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C21" s="9"/>
       <c r="D21" s="10"/>
       <c r="E21" s="10"/>
@@ -4180,7 +4180,7 @@
       <c r="O21" s="10"/>
       <c r="P21" s="11"/>
     </row>
-    <row r="22" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C22" s="9"/>
       <c r="D22" s="10"/>
       <c r="E22" s="10"/>
@@ -4196,7 +4196,7 @@
       <c r="O22" s="10"/>
       <c r="P22" s="11"/>
     </row>
-    <row r="23" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C23" s="9"/>
       <c r="D23" s="10"/>
       <c r="E23" s="10"/>
@@ -4212,7 +4212,7 @@
       <c r="O23" s="10"/>
       <c r="P23" s="11"/>
     </row>
-    <row r="24" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C24" s="9"/>
       <c r="D24" s="10"/>
       <c r="E24" s="10"/>
@@ -4228,7 +4228,7 @@
       <c r="O24" s="10"/>
       <c r="P24" s="11"/>
     </row>
-    <row r="25" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C25" s="9"/>
       <c r="D25" s="10"/>
       <c r="E25" s="10"/>
@@ -4244,7 +4244,7 @@
       <c r="O25" s="10"/>
       <c r="P25" s="11"/>
     </row>
-    <row r="26" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C26" s="9"/>
       <c r="D26" s="10"/>
       <c r="E26" s="10"/>
@@ -4260,7 +4260,7 @@
       <c r="O26" s="10"/>
       <c r="P26" s="11"/>
     </row>
-    <row r="27" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C27" s="9"/>
       <c r="D27" s="10"/>
       <c r="E27" s="10"/>
@@ -4276,7 +4276,7 @@
       <c r="O27" s="10"/>
       <c r="P27" s="11"/>
     </row>
-    <row r="28" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C28" s="9"/>
       <c r="D28" s="10"/>
       <c r="E28" s="10"/>
@@ -4292,7 +4292,7 @@
       <c r="O28" s="10"/>
       <c r="P28" s="11"/>
     </row>
-    <row r="29" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C29" s="9"/>
       <c r="D29" s="10"/>
       <c r="E29" s="10"/>
@@ -4308,7 +4308,7 @@
       <c r="O29" s="10"/>
       <c r="P29" s="11"/>
     </row>
-    <row r="30" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="3:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C30" s="12"/>
       <c r="D30" s="13"/>
       <c r="E30" s="13"/>
@@ -4340,13 +4340,13 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" customWidth="1"/>
-    <col min="2" max="2" width="25.7109375" customWidth="1"/>
+    <col min="1" max="1" width="10.7265625" customWidth="1"/>
+    <col min="2" max="2" width="25.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="17" t="s">
         <v>220</v>
       </c>
@@ -4366,7 +4366,7 @@
       <c r="O1" s="7"/>
       <c r="P1" s="8"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>219</v>
       </c>
@@ -4388,7 +4388,7 @@
       <c r="O2" s="10"/>
       <c r="P2" s="11"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3" s="4"/>
       <c r="B3" s="5"/>
       <c r="C3" s="9"/>
@@ -4406,7 +4406,7 @@
       <c r="O3" s="10"/>
       <c r="P3" s="11"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C4" s="9"/>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -4422,7 +4422,7 @@
       <c r="O4" s="10"/>
       <c r="P4" s="11"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C5" s="9"/>
       <c r="D5" s="10"/>
       <c r="E5" s="10"/>
@@ -4438,7 +4438,7 @@
       <c r="O5" s="10"/>
       <c r="P5" s="11"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C6" s="9"/>
       <c r="D6" s="10"/>
       <c r="E6" s="10"/>
@@ -4454,7 +4454,7 @@
       <c r="O6" s="10"/>
       <c r="P6" s="11"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C7" s="9"/>
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
@@ -4470,7 +4470,7 @@
       <c r="O7" s="10"/>
       <c r="P7" s="11"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C8" s="9"/>
       <c r="D8" s="10"/>
       <c r="E8" s="10"/>
@@ -4486,7 +4486,7 @@
       <c r="O8" s="10"/>
       <c r="P8" s="11"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C9" s="9"/>
       <c r="D9" s="10"/>
       <c r="E9" s="10"/>
@@ -4502,7 +4502,7 @@
       <c r="O9" s="10"/>
       <c r="P9" s="11"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C10" s="9"/>
       <c r="D10" s="10"/>
       <c r="E10" s="10"/>
@@ -4518,7 +4518,7 @@
       <c r="O10" s="10"/>
       <c r="P10" s="11"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C11" s="9"/>
       <c r="D11" s="10"/>
       <c r="E11" s="10"/>
@@ -4534,7 +4534,7 @@
       <c r="O11" s="10"/>
       <c r="P11" s="11"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C12" s="9"/>
       <c r="D12" s="10"/>
       <c r="E12" s="10"/>
@@ -4550,7 +4550,7 @@
       <c r="O12" s="10"/>
       <c r="P12" s="11"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C13" s="9"/>
       <c r="D13" s="10"/>
       <c r="E13" s="10"/>
@@ -4566,7 +4566,7 @@
       <c r="O13" s="10"/>
       <c r="P13" s="11"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C14" s="9"/>
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
@@ -4582,7 +4582,7 @@
       <c r="O14" s="10"/>
       <c r="P14" s="11"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C15" s="9"/>
       <c r="D15" s="10"/>
       <c r="E15" s="10"/>
@@ -4598,7 +4598,7 @@
       <c r="O15" s="10"/>
       <c r="P15" s="11"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C16" s="9"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
@@ -4614,7 +4614,7 @@
       <c r="O16" s="10"/>
       <c r="P16" s="11"/>
     </row>
-    <row r="17" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C17" s="9"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
@@ -4630,7 +4630,7 @@
       <c r="O17" s="10"/>
       <c r="P17" s="11"/>
     </row>
-    <row r="18" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C18" s="9"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
@@ -4646,7 +4646,7 @@
       <c r="O18" s="10"/>
       <c r="P18" s="11"/>
     </row>
-    <row r="19" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C19" s="9"/>
       <c r="D19" s="10"/>
       <c r="E19" s="10"/>
@@ -4662,7 +4662,7 @@
       <c r="O19" s="10"/>
       <c r="P19" s="11"/>
     </row>
-    <row r="20" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C20" s="9"/>
       <c r="D20" s="10"/>
       <c r="E20" s="10"/>
@@ -4678,7 +4678,7 @@
       <c r="O20" s="10"/>
       <c r="P20" s="11"/>
     </row>
-    <row r="21" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C21" s="9"/>
       <c r="D21" s="10"/>
       <c r="E21" s="10"/>
@@ -4694,7 +4694,7 @@
       <c r="O21" s="10"/>
       <c r="P21" s="11"/>
     </row>
-    <row r="22" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C22" s="9"/>
       <c r="D22" s="10"/>
       <c r="E22" s="10"/>
@@ -4710,7 +4710,7 @@
       <c r="O22" s="10"/>
       <c r="P22" s="11"/>
     </row>
-    <row r="23" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C23" s="9"/>
       <c r="D23" s="10"/>
       <c r="E23" s="10"/>
@@ -4726,7 +4726,7 @@
       <c r="O23" s="10"/>
       <c r="P23" s="11"/>
     </row>
-    <row r="24" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C24" s="9"/>
       <c r="D24" s="10"/>
       <c r="E24" s="10"/>
@@ -4742,7 +4742,7 @@
       <c r="O24" s="10"/>
       <c r="P24" s="11"/>
     </row>
-    <row r="25" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C25" s="9"/>
       <c r="D25" s="10"/>
       <c r="E25" s="10"/>
@@ -4758,7 +4758,7 @@
       <c r="O25" s="10"/>
       <c r="P25" s="11"/>
     </row>
-    <row r="26" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C26" s="9"/>
       <c r="D26" s="10"/>
       <c r="E26" s="10"/>
@@ -4774,7 +4774,7 @@
       <c r="O26" s="10"/>
       <c r="P26" s="11"/>
     </row>
-    <row r="27" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C27" s="9"/>
       <c r="D27" s="10"/>
       <c r="E27" s="10"/>
@@ -4790,7 +4790,7 @@
       <c r="O27" s="10"/>
       <c r="P27" s="11"/>
     </row>
-    <row r="28" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C28" s="9"/>
       <c r="D28" s="10"/>
       <c r="E28" s="10"/>
@@ -4806,7 +4806,7 @@
       <c r="O28" s="10"/>
       <c r="P28" s="11"/>
     </row>
-    <row r="29" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C29" s="9"/>
       <c r="D29" s="10"/>
       <c r="E29" s="10"/>
@@ -4822,7 +4822,7 @@
       <c r="O29" s="10"/>
       <c r="P29" s="11"/>
     </row>
-    <row r="30" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="3:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C30" s="12"/>
       <c r="D30" s="13"/>
       <c r="E30" s="13"/>
@@ -4854,13 +4854,13 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" customWidth="1"/>
-    <col min="2" max="2" width="25.7109375" customWidth="1"/>
+    <col min="1" max="1" width="10.7265625" customWidth="1"/>
+    <col min="2" max="2" width="25.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="17" t="s">
         <v>220</v>
       </c>
@@ -4880,7 +4880,7 @@
       <c r="O1" s="7"/>
       <c r="P1" s="8"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>219</v>
       </c>
@@ -4902,7 +4902,7 @@
       <c r="O2" s="10"/>
       <c r="P2" s="11"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3" s="4"/>
       <c r="B3" s="5"/>
       <c r="C3" s="9"/>
@@ -4920,7 +4920,7 @@
       <c r="O3" s="10"/>
       <c r="P3" s="11"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C4" s="9"/>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -4936,7 +4936,7 @@
       <c r="O4" s="10"/>
       <c r="P4" s="11"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C5" s="9"/>
       <c r="D5" s="10"/>
       <c r="E5" s="10"/>
@@ -4952,7 +4952,7 @@
       <c r="O5" s="10"/>
       <c r="P5" s="11"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C6" s="9"/>
       <c r="D6" s="10"/>
       <c r="E6" s="10"/>
@@ -4968,7 +4968,7 @@
       <c r="O6" s="10"/>
       <c r="P6" s="11"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C7" s="9"/>
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
@@ -4984,7 +4984,7 @@
       <c r="O7" s="10"/>
       <c r="P7" s="11"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C8" s="9"/>
       <c r="D8" s="10"/>
       <c r="E8" s="10"/>
@@ -5000,7 +5000,7 @@
       <c r="O8" s="10"/>
       <c r="P8" s="11"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C9" s="9"/>
       <c r="D9" s="10"/>
       <c r="E9" s="10"/>
@@ -5016,7 +5016,7 @@
       <c r="O9" s="10"/>
       <c r="P9" s="11"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C10" s="9"/>
       <c r="D10" s="10"/>
       <c r="E10" s="10"/>
@@ -5032,7 +5032,7 @@
       <c r="O10" s="10"/>
       <c r="P10" s="11"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C11" s="9"/>
       <c r="D11" s="10"/>
       <c r="E11" s="10"/>
@@ -5048,7 +5048,7 @@
       <c r="O11" s="10"/>
       <c r="P11" s="11"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C12" s="9"/>
       <c r="D12" s="10"/>
       <c r="E12" s="10"/>
@@ -5064,7 +5064,7 @@
       <c r="O12" s="10"/>
       <c r="P12" s="11"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C13" s="9"/>
       <c r="D13" s="10"/>
       <c r="E13" s="10"/>
@@ -5080,7 +5080,7 @@
       <c r="O13" s="10"/>
       <c r="P13" s="11"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C14" s="9"/>
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
@@ -5096,7 +5096,7 @@
       <c r="O14" s="10"/>
       <c r="P14" s="11"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C15" s="9"/>
       <c r="D15" s="10"/>
       <c r="E15" s="10"/>
@@ -5112,7 +5112,7 @@
       <c r="O15" s="10"/>
       <c r="P15" s="11"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C16" s="9"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
@@ -5128,7 +5128,7 @@
       <c r="O16" s="10"/>
       <c r="P16" s="11"/>
     </row>
-    <row r="17" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C17" s="9"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
@@ -5144,7 +5144,7 @@
       <c r="O17" s="10"/>
       <c r="P17" s="11"/>
     </row>
-    <row r="18" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C18" s="9"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
@@ -5160,7 +5160,7 @@
       <c r="O18" s="10"/>
       <c r="P18" s="11"/>
     </row>
-    <row r="19" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C19" s="9"/>
       <c r="D19" s="10"/>
       <c r="E19" s="10"/>
@@ -5176,7 +5176,7 @@
       <c r="O19" s="10"/>
       <c r="P19" s="11"/>
     </row>
-    <row r="20" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C20" s="9"/>
       <c r="D20" s="10"/>
       <c r="E20" s="10"/>
@@ -5192,7 +5192,7 @@
       <c r="O20" s="10"/>
       <c r="P20" s="11"/>
     </row>
-    <row r="21" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C21" s="9"/>
       <c r="D21" s="10"/>
       <c r="E21" s="10"/>
@@ -5208,7 +5208,7 @@
       <c r="O21" s="10"/>
       <c r="P21" s="11"/>
     </row>
-    <row r="22" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C22" s="9"/>
       <c r="D22" s="10"/>
       <c r="E22" s="10"/>
@@ -5224,7 +5224,7 @@
       <c r="O22" s="10"/>
       <c r="P22" s="11"/>
     </row>
-    <row r="23" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C23" s="9"/>
       <c r="D23" s="10"/>
       <c r="E23" s="10"/>
@@ -5240,7 +5240,7 @@
       <c r="O23" s="10"/>
       <c r="P23" s="11"/>
     </row>
-    <row r="24" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C24" s="9"/>
       <c r="D24" s="10"/>
       <c r="E24" s="10"/>
@@ -5256,7 +5256,7 @@
       <c r="O24" s="10"/>
       <c r="P24" s="11"/>
     </row>
-    <row r="25" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C25" s="9"/>
       <c r="D25" s="10"/>
       <c r="E25" s="10"/>
@@ -5272,7 +5272,7 @@
       <c r="O25" s="10"/>
       <c r="P25" s="11"/>
     </row>
-    <row r="26" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C26" s="9"/>
       <c r="D26" s="10"/>
       <c r="E26" s="10"/>
@@ -5288,7 +5288,7 @@
       <c r="O26" s="10"/>
       <c r="P26" s="11"/>
     </row>
-    <row r="27" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C27" s="9"/>
       <c r="D27" s="10"/>
       <c r="E27" s="10"/>
@@ -5304,7 +5304,7 @@
       <c r="O27" s="10"/>
       <c r="P27" s="11"/>
     </row>
-    <row r="28" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C28" s="9"/>
       <c r="D28" s="10"/>
       <c r="E28" s="10"/>
@@ -5320,7 +5320,7 @@
       <c r="O28" s="10"/>
       <c r="P28" s="11"/>
     </row>
-    <row r="29" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C29" s="9"/>
       <c r="D29" s="10"/>
       <c r="E29" s="10"/>
@@ -5336,7 +5336,7 @@
       <c r="O29" s="10"/>
       <c r="P29" s="11"/>
     </row>
-    <row r="30" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="3:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C30" s="12"/>
       <c r="D30" s="13"/>
       <c r="E30" s="13"/>
@@ -5368,13 +5368,13 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" customWidth="1"/>
-    <col min="2" max="2" width="25.7109375" customWidth="1"/>
+    <col min="1" max="1" width="10.7265625" customWidth="1"/>
+    <col min="2" max="2" width="25.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="17" t="s">
         <v>220</v>
       </c>
@@ -5394,7 +5394,7 @@
       <c r="O1" s="7"/>
       <c r="P1" s="8"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>219</v>
       </c>
@@ -5416,7 +5416,7 @@
       <c r="O2" s="10"/>
       <c r="P2" s="11"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3" s="4"/>
       <c r="B3" s="5"/>
       <c r="C3" s="9"/>
@@ -5434,7 +5434,7 @@
       <c r="O3" s="10"/>
       <c r="P3" s="11"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C4" s="9"/>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -5450,7 +5450,7 @@
       <c r="O4" s="10"/>
       <c r="P4" s="11"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C5" s="9"/>
       <c r="D5" s="10"/>
       <c r="E5" s="10"/>
@@ -5466,7 +5466,7 @@
       <c r="O5" s="10"/>
       <c r="P5" s="11"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C6" s="9"/>
       <c r="D6" s="10"/>
       <c r="E6" s="10"/>
@@ -5482,7 +5482,7 @@
       <c r="O6" s="10"/>
       <c r="P6" s="11"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C7" s="9"/>
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
@@ -5498,7 +5498,7 @@
       <c r="O7" s="10"/>
       <c r="P7" s="11"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C8" s="9"/>
       <c r="D8" s="10"/>
       <c r="E8" s="10"/>
@@ -5514,7 +5514,7 @@
       <c r="O8" s="10"/>
       <c r="P8" s="11"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C9" s="9"/>
       <c r="D9" s="10"/>
       <c r="E9" s="10"/>
@@ -5530,7 +5530,7 @@
       <c r="O9" s="10"/>
       <c r="P9" s="11"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C10" s="9"/>
       <c r="D10" s="10"/>
       <c r="E10" s="10"/>
@@ -5546,7 +5546,7 @@
       <c r="O10" s="10"/>
       <c r="P10" s="11"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C11" s="9"/>
       <c r="D11" s="10"/>
       <c r="E11" s="10"/>
@@ -5562,7 +5562,7 @@
       <c r="O11" s="10"/>
       <c r="P11" s="11"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C12" s="9"/>
       <c r="D12" s="10"/>
       <c r="E12" s="10"/>
@@ -5578,7 +5578,7 @@
       <c r="O12" s="10"/>
       <c r="P12" s="11"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C13" s="9"/>
       <c r="D13" s="10"/>
       <c r="E13" s="10"/>
@@ -5594,7 +5594,7 @@
       <c r="O13" s="10"/>
       <c r="P13" s="11"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C14" s="9"/>
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
@@ -5610,7 +5610,7 @@
       <c r="O14" s="10"/>
       <c r="P14" s="11"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C15" s="9"/>
       <c r="D15" s="10"/>
       <c r="E15" s="10"/>
@@ -5626,7 +5626,7 @@
       <c r="O15" s="10"/>
       <c r="P15" s="11"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C16" s="9"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
@@ -5642,7 +5642,7 @@
       <c r="O16" s="10"/>
       <c r="P16" s="11"/>
     </row>
-    <row r="17" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C17" s="9"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
@@ -5658,7 +5658,7 @@
       <c r="O17" s="10"/>
       <c r="P17" s="11"/>
     </row>
-    <row r="18" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C18" s="9"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
@@ -5674,7 +5674,7 @@
       <c r="O18" s="10"/>
       <c r="P18" s="11"/>
     </row>
-    <row r="19" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C19" s="9"/>
       <c r="D19" s="10"/>
       <c r="E19" s="10"/>
@@ -5690,7 +5690,7 @@
       <c r="O19" s="10"/>
       <c r="P19" s="11"/>
     </row>
-    <row r="20" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C20" s="9"/>
       <c r="D20" s="10"/>
       <c r="E20" s="10"/>
@@ -5706,7 +5706,7 @@
       <c r="O20" s="10"/>
       <c r="P20" s="11"/>
     </row>
-    <row r="21" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C21" s="9"/>
       <c r="D21" s="10"/>
       <c r="E21" s="10"/>
@@ -5722,7 +5722,7 @@
       <c r="O21" s="10"/>
       <c r="P21" s="11"/>
     </row>
-    <row r="22" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C22" s="9"/>
       <c r="D22" s="10"/>
       <c r="E22" s="10"/>
@@ -5738,7 +5738,7 @@
       <c r="O22" s="10"/>
       <c r="P22" s="11"/>
     </row>
-    <row r="23" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C23" s="9"/>
       <c r="D23" s="10"/>
       <c r="E23" s="10"/>
@@ -5754,7 +5754,7 @@
       <c r="O23" s="10"/>
       <c r="P23" s="11"/>
     </row>
-    <row r="24" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C24" s="9"/>
       <c r="D24" s="10"/>
       <c r="E24" s="10"/>
@@ -5770,7 +5770,7 @@
       <c r="O24" s="10"/>
       <c r="P24" s="11"/>
     </row>
-    <row r="25" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C25" s="9"/>
       <c r="D25" s="10"/>
       <c r="E25" s="10"/>
@@ -5786,7 +5786,7 @@
       <c r="O25" s="10"/>
       <c r="P25" s="11"/>
     </row>
-    <row r="26" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C26" s="9"/>
       <c r="D26" s="10"/>
       <c r="E26" s="10"/>
@@ -5802,7 +5802,7 @@
       <c r="O26" s="10"/>
       <c r="P26" s="11"/>
     </row>
-    <row r="27" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C27" s="9"/>
       <c r="D27" s="10"/>
       <c r="E27" s="10"/>
@@ -5818,7 +5818,7 @@
       <c r="O27" s="10"/>
       <c r="P27" s="11"/>
     </row>
-    <row r="28" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C28" s="9"/>
       <c r="D28" s="10"/>
       <c r="E28" s="10"/>
@@ -5834,7 +5834,7 @@
       <c r="O28" s="10"/>
       <c r="P28" s="11"/>
     </row>
-    <row r="29" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C29" s="9"/>
       <c r="D29" s="10"/>
       <c r="E29" s="10"/>
@@ -5850,7 +5850,7 @@
       <c r="O29" s="10"/>
       <c r="P29" s="11"/>
     </row>
-    <row r="30" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="3:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C30" s="12"/>
       <c r="D30" s="13"/>
       <c r="E30" s="13"/>
@@ -5882,13 +5882,13 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" customWidth="1"/>
-    <col min="2" max="2" width="25.7109375" customWidth="1"/>
+    <col min="1" max="1" width="10.7265625" customWidth="1"/>
+    <col min="2" max="2" width="25.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="17" t="s">
         <v>220</v>
       </c>
@@ -5908,7 +5908,7 @@
       <c r="O1" s="7"/>
       <c r="P1" s="8"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>219</v>
       </c>
@@ -5930,7 +5930,7 @@
       <c r="O2" s="10"/>
       <c r="P2" s="11"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3" s="4"/>
       <c r="B3" s="5"/>
       <c r="C3" s="9"/>
@@ -5948,7 +5948,7 @@
       <c r="O3" s="10"/>
       <c r="P3" s="11"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C4" s="9"/>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -5964,7 +5964,7 @@
       <c r="O4" s="10"/>
       <c r="P4" s="11"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C5" s="9"/>
       <c r="D5" s="10"/>
       <c r="E5" s="10"/>
@@ -5980,7 +5980,7 @@
       <c r="O5" s="10"/>
       <c r="P5" s="11"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C6" s="9"/>
       <c r="D6" s="10"/>
       <c r="E6" s="10"/>
@@ -5996,7 +5996,7 @@
       <c r="O6" s="10"/>
       <c r="P6" s="11"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C7" s="9"/>
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
@@ -6012,7 +6012,7 @@
       <c r="O7" s="10"/>
       <c r="P7" s="11"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C8" s="9"/>
       <c r="D8" s="10"/>
       <c r="E8" s="10"/>
@@ -6028,7 +6028,7 @@
       <c r="O8" s="10"/>
       <c r="P8" s="11"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C9" s="9"/>
       <c r="D9" s="10"/>
       <c r="E9" s="10"/>
@@ -6044,7 +6044,7 @@
       <c r="O9" s="10"/>
       <c r="P9" s="11"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C10" s="9"/>
       <c r="D10" s="10"/>
       <c r="E10" s="10"/>
@@ -6060,7 +6060,7 @@
       <c r="O10" s="10"/>
       <c r="P10" s="11"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C11" s="9"/>
       <c r="D11" s="10"/>
       <c r="E11" s="10"/>
@@ -6076,7 +6076,7 @@
       <c r="O11" s="10"/>
       <c r="P11" s="11"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C12" s="9"/>
       <c r="D12" s="10"/>
       <c r="E12" s="10"/>
@@ -6092,7 +6092,7 @@
       <c r="O12" s="10"/>
       <c r="P12" s="11"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C13" s="9"/>
       <c r="D13" s="10"/>
       <c r="E13" s="10"/>
@@ -6108,7 +6108,7 @@
       <c r="O13" s="10"/>
       <c r="P13" s="11"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C14" s="9"/>
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
@@ -6124,7 +6124,7 @@
       <c r="O14" s="10"/>
       <c r="P14" s="11"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C15" s="9"/>
       <c r="D15" s="10"/>
       <c r="E15" s="10"/>
@@ -6140,7 +6140,7 @@
       <c r="O15" s="10"/>
       <c r="P15" s="11"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C16" s="9"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
@@ -6156,7 +6156,7 @@
       <c r="O16" s="10"/>
       <c r="P16" s="11"/>
     </row>
-    <row r="17" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C17" s="9"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
@@ -6172,7 +6172,7 @@
       <c r="O17" s="10"/>
       <c r="P17" s="11"/>
     </row>
-    <row r="18" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C18" s="9"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
@@ -6188,7 +6188,7 @@
       <c r="O18" s="10"/>
       <c r="P18" s="11"/>
     </row>
-    <row r="19" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C19" s="9"/>
       <c r="D19" s="10"/>
       <c r="E19" s="10"/>
@@ -6204,7 +6204,7 @@
       <c r="O19" s="10"/>
       <c r="P19" s="11"/>
     </row>
-    <row r="20" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C20" s="9"/>
       <c r="D20" s="10"/>
       <c r="E20" s="10"/>
@@ -6220,7 +6220,7 @@
       <c r="O20" s="10"/>
       <c r="P20" s="11"/>
     </row>
-    <row r="21" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C21" s="9"/>
       <c r="D21" s="10"/>
       <c r="E21" s="10"/>
@@ -6236,7 +6236,7 @@
       <c r="O21" s="10"/>
       <c r="P21" s="11"/>
     </row>
-    <row r="22" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C22" s="9"/>
       <c r="D22" s="10"/>
       <c r="E22" s="10"/>
@@ -6252,7 +6252,7 @@
       <c r="O22" s="10"/>
       <c r="P22" s="11"/>
     </row>
-    <row r="23" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C23" s="9"/>
       <c r="D23" s="10"/>
       <c r="E23" s="10"/>
@@ -6268,7 +6268,7 @@
       <c r="O23" s="10"/>
       <c r="P23" s="11"/>
     </row>
-    <row r="24" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C24" s="9"/>
       <c r="D24" s="10"/>
       <c r="E24" s="10"/>
@@ -6284,7 +6284,7 @@
       <c r="O24" s="10"/>
       <c r="P24" s="11"/>
     </row>
-    <row r="25" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C25" s="9"/>
       <c r="D25" s="10"/>
       <c r="E25" s="10"/>
@@ -6300,7 +6300,7 @@
       <c r="O25" s="10"/>
       <c r="P25" s="11"/>
     </row>
-    <row r="26" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C26" s="9"/>
       <c r="D26" s="10"/>
       <c r="E26" s="10"/>
@@ -6316,7 +6316,7 @@
       <c r="O26" s="10"/>
       <c r="P26" s="11"/>
     </row>
-    <row r="27" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C27" s="9"/>
       <c r="D27" s="10"/>
       <c r="E27" s="10"/>
@@ -6332,7 +6332,7 @@
       <c r="O27" s="10"/>
       <c r="P27" s="11"/>
     </row>
-    <row r="28" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C28" s="9"/>
       <c r="D28" s="10"/>
       <c r="E28" s="10"/>
@@ -6348,7 +6348,7 @@
       <c r="O28" s="10"/>
       <c r="P28" s="11"/>
     </row>
-    <row r="29" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C29" s="9"/>
       <c r="D29" s="10"/>
       <c r="E29" s="10"/>
@@ -6364,7 +6364,7 @@
       <c r="O29" s="10"/>
       <c r="P29" s="11"/>
     </row>
-    <row r="30" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="3:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C30" s="12"/>
       <c r="D30" s="13"/>
       <c r="E30" s="13"/>
@@ -6396,13 +6396,13 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" customWidth="1"/>
-    <col min="2" max="2" width="25.7109375" customWidth="1"/>
+    <col min="1" max="1" width="10.7265625" customWidth="1"/>
+    <col min="2" max="2" width="25.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="17" t="s">
         <v>220</v>
       </c>
@@ -6422,7 +6422,7 @@
       <c r="O1" s="7"/>
       <c r="P1" s="8"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>219</v>
       </c>
@@ -6444,7 +6444,7 @@
       <c r="O2" s="10"/>
       <c r="P2" s="11"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3" s="4"/>
       <c r="B3" s="5"/>
       <c r="C3" s="9"/>
@@ -6462,7 +6462,7 @@
       <c r="O3" s="10"/>
       <c r="P3" s="11"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C4" s="9"/>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -6478,7 +6478,7 @@
       <c r="O4" s="10"/>
       <c r="P4" s="11"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C5" s="9"/>
       <c r="D5" s="10"/>
       <c r="E5" s="10"/>
@@ -6494,7 +6494,7 @@
       <c r="O5" s="10"/>
       <c r="P5" s="11"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C6" s="9"/>
       <c r="D6" s="10"/>
       <c r="E6" s="10"/>
@@ -6510,7 +6510,7 @@
       <c r="O6" s="10"/>
       <c r="P6" s="11"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C7" s="9"/>
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
@@ -6526,7 +6526,7 @@
       <c r="O7" s="10"/>
       <c r="P7" s="11"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C8" s="9"/>
       <c r="D8" s="10"/>
       <c r="E8" s="10"/>
@@ -6542,7 +6542,7 @@
       <c r="O8" s="10"/>
       <c r="P8" s="11"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C9" s="9"/>
       <c r="D9" s="10"/>
       <c r="E9" s="10"/>
@@ -6558,7 +6558,7 @@
       <c r="O9" s="10"/>
       <c r="P9" s="11"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C10" s="9"/>
       <c r="D10" s="10"/>
       <c r="E10" s="10"/>
@@ -6574,7 +6574,7 @@
       <c r="O10" s="10"/>
       <c r="P10" s="11"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C11" s="9"/>
       <c r="D11" s="10"/>
       <c r="E11" s="10"/>
@@ -6590,7 +6590,7 @@
       <c r="O11" s="10"/>
       <c r="P11" s="11"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C12" s="9"/>
       <c r="D12" s="10"/>
       <c r="E12" s="10"/>
@@ -6606,7 +6606,7 @@
       <c r="O12" s="10"/>
       <c r="P12" s="11"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C13" s="9"/>
       <c r="D13" s="10"/>
       <c r="E13" s="10"/>
@@ -6622,7 +6622,7 @@
       <c r="O13" s="10"/>
       <c r="P13" s="11"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C14" s="9"/>
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
@@ -6638,7 +6638,7 @@
       <c r="O14" s="10"/>
       <c r="P14" s="11"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C15" s="9"/>
       <c r="D15" s="10"/>
       <c r="E15" s="10"/>
@@ -6654,7 +6654,7 @@
       <c r="O15" s="10"/>
       <c r="P15" s="11"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C16" s="9"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
@@ -6670,7 +6670,7 @@
       <c r="O16" s="10"/>
       <c r="P16" s="11"/>
     </row>
-    <row r="17" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C17" s="9"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
@@ -6686,7 +6686,7 @@
       <c r="O17" s="10"/>
       <c r="P17" s="11"/>
     </row>
-    <row r="18" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C18" s="9"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
@@ -6702,7 +6702,7 @@
       <c r="O18" s="10"/>
       <c r="P18" s="11"/>
     </row>
-    <row r="19" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C19" s="9"/>
       <c r="D19" s="10"/>
       <c r="E19" s="10"/>
@@ -6718,7 +6718,7 @@
       <c r="O19" s="10"/>
       <c r="P19" s="11"/>
     </row>
-    <row r="20" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C20" s="9"/>
       <c r="D20" s="10"/>
       <c r="E20" s="10"/>
@@ -6734,7 +6734,7 @@
       <c r="O20" s="10"/>
       <c r="P20" s="11"/>
     </row>
-    <row r="21" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C21" s="9"/>
       <c r="D21" s="10"/>
       <c r="E21" s="10"/>
@@ -6750,7 +6750,7 @@
       <c r="O21" s="10"/>
       <c r="P21" s="11"/>
     </row>
-    <row r="22" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C22" s="9"/>
       <c r="D22" s="10"/>
       <c r="E22" s="10"/>
@@ -6766,7 +6766,7 @@
       <c r="O22" s="10"/>
       <c r="P22" s="11"/>
     </row>
-    <row r="23" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C23" s="9"/>
       <c r="D23" s="10"/>
       <c r="E23" s="10"/>
@@ -6782,7 +6782,7 @@
       <c r="O23" s="10"/>
       <c r="P23" s="11"/>
     </row>
-    <row r="24" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C24" s="9"/>
       <c r="D24" s="10"/>
       <c r="E24" s="10"/>
@@ -6798,7 +6798,7 @@
       <c r="O24" s="10"/>
       <c r="P24" s="11"/>
     </row>
-    <row r="25" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C25" s="9"/>
       <c r="D25" s="10"/>
       <c r="E25" s="10"/>
@@ -6814,7 +6814,7 @@
       <c r="O25" s="10"/>
       <c r="P25" s="11"/>
     </row>
-    <row r="26" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C26" s="9"/>
       <c r="D26" s="10"/>
       <c r="E26" s="10"/>
@@ -6830,7 +6830,7 @@
       <c r="O26" s="10"/>
       <c r="P26" s="11"/>
     </row>
-    <row r="27" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C27" s="9"/>
       <c r="D27" s="10"/>
       <c r="E27" s="10"/>
@@ -6846,7 +6846,7 @@
       <c r="O27" s="10"/>
       <c r="P27" s="11"/>
     </row>
-    <row r="28" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C28" s="9"/>
       <c r="D28" s="10"/>
       <c r="E28" s="10"/>
@@ -6862,7 +6862,7 @@
       <c r="O28" s="10"/>
       <c r="P28" s="11"/>
     </row>
-    <row r="29" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C29" s="9"/>
       <c r="D29" s="10"/>
       <c r="E29" s="10"/>
@@ -6878,7 +6878,7 @@
       <c r="O29" s="10"/>
       <c r="P29" s="11"/>
     </row>
-    <row r="30" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="3:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C30" s="12"/>
       <c r="D30" s="13"/>
       <c r="E30" s="13"/>
@@ -6911,33 +6911,33 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.140625" customWidth="1"/>
+    <col min="1" max="1" width="18.1796875" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
     <col min="3" max="3" width="12" customWidth="1"/>
-    <col min="4" max="5" width="20.140625" customWidth="1"/>
-    <col min="6" max="6" width="17.7109375" customWidth="1"/>
-    <col min="7" max="7" width="23.28515625" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" customWidth="1"/>
-    <col min="9" max="9" width="10.85546875" customWidth="1"/>
-    <col min="11" max="11" width="15.85546875" customWidth="1"/>
-    <col min="12" max="12" width="17.85546875" customWidth="1"/>
-    <col min="13" max="13" width="11.85546875" customWidth="1"/>
-    <col min="14" max="14" width="22.140625" customWidth="1"/>
-    <col min="15" max="15" width="11.140625" customWidth="1"/>
+    <col min="4" max="5" width="20.1796875" customWidth="1"/>
+    <col min="6" max="6" width="17.7265625" customWidth="1"/>
+    <col min="7" max="7" width="23.26953125" customWidth="1"/>
+    <col min="8" max="8" width="11.1796875" customWidth="1"/>
+    <col min="9" max="9" width="10.81640625" customWidth="1"/>
+    <col min="11" max="11" width="15.81640625" customWidth="1"/>
+    <col min="12" max="12" width="17.81640625" customWidth="1"/>
+    <col min="13" max="13" width="11.81640625" customWidth="1"/>
+    <col min="14" max="14" width="22.1796875" customWidth="1"/>
+    <col min="15" max="15" width="11.1796875" customWidth="1"/>
     <col min="16" max="16" width="11" customWidth="1"/>
     <col min="17" max="17" width="13" customWidth="1"/>
-    <col min="19" max="19" width="26.7109375" customWidth="1"/>
-    <col min="20" max="20" width="15.85546875" customWidth="1"/>
-    <col min="21" max="21" width="16.7109375" customWidth="1"/>
-    <col min="22" max="22" width="17.5703125" customWidth="1"/>
+    <col min="19" max="19" width="26.7265625" customWidth="1"/>
+    <col min="20" max="20" width="15.81640625" customWidth="1"/>
+    <col min="21" max="21" width="16.7265625" customWidth="1"/>
+    <col min="22" max="22" width="17.54296875" customWidth="1"/>
     <col min="23" max="23" width="16" customWidth="1"/>
     <col min="27" max="27" width="16" customWidth="1"/>
-    <col min="31" max="31" width="16.5703125" customWidth="1"/>
+    <col min="31" max="31" width="16.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -7032,7 +7032,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>90</v>
       </c>
@@ -7100,7 +7100,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>90</v>
       </c>
@@ -7185,28 +7185,28 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.140625" customWidth="1"/>
+    <col min="1" max="1" width="17.1796875" customWidth="1"/>
     <col min="2" max="3" width="19" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" customWidth="1"/>
-    <col min="6" max="7" width="16.5703125" customWidth="1"/>
+    <col min="4" max="4" width="10.81640625" customWidth="1"/>
+    <col min="5" max="5" width="14.453125" customWidth="1"/>
+    <col min="6" max="7" width="16.54296875" customWidth="1"/>
     <col min="8" max="8" width="18" customWidth="1"/>
-    <col min="9" max="10" width="16.140625" customWidth="1"/>
-    <col min="11" max="11" width="17.5703125" customWidth="1"/>
+    <col min="9" max="10" width="16.1796875" customWidth="1"/>
+    <col min="11" max="11" width="17.54296875" customWidth="1"/>
     <col min="12" max="12" width="16" customWidth="1"/>
-    <col min="13" max="13" width="16.42578125" customWidth="1"/>
-    <col min="14" max="14" width="19.140625" customWidth="1"/>
-    <col min="15" max="15" width="17.85546875" customWidth="1"/>
-    <col min="16" max="16" width="15.28515625" customWidth="1"/>
-    <col min="17" max="17" width="13.42578125" customWidth="1"/>
-    <col min="20" max="20" width="18.28515625" customWidth="1"/>
-    <col min="23" max="23" width="16.7109375" customWidth="1"/>
-    <col min="24" max="24" width="13.5703125" customWidth="1"/>
+    <col min="13" max="13" width="16.453125" customWidth="1"/>
+    <col min="14" max="14" width="19.1796875" customWidth="1"/>
+    <col min="15" max="15" width="17.81640625" customWidth="1"/>
+    <col min="16" max="16" width="15.26953125" customWidth="1"/>
+    <col min="17" max="17" width="13.453125" customWidth="1"/>
+    <col min="20" max="20" width="18.26953125" customWidth="1"/>
+    <col min="23" max="23" width="16.7265625" customWidth="1"/>
+    <col min="24" max="24" width="13.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" ht="31" x14ac:dyDescent="0.35">
       <c r="A1" s="2">
         <v>2025</v>
       </c>
@@ -7215,7 +7215,7 @@
       </c>
       <c r="C1" s="2"/>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>154</v>
       </c>
@@ -7306,9 +7306,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>117</v>
       </c>
@@ -7346,7 +7346,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>0.01</v>
       </c>
@@ -7399,24 +7399,24 @@
   </sheetPr>
   <dimension ref="A1:Z93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="29.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="11.7109375" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" style="3"/>
-    <col min="10" max="10" width="9.140625" style="3"/>
+    <col min="1" max="1" width="29.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="11.7265625" customWidth="1"/>
+    <col min="6" max="6" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.1796875" style="3"/>
+    <col min="10" max="10" width="9.1796875" style="3"/>
     <col min="11" max="11" width="15" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="39.28515625" customWidth="1"/>
-    <col min="13" max="26" width="9.140625" style="3"/>
+    <col min="12" max="12" width="39.26953125" customWidth="1"/>
+    <col min="13" max="26" width="9.1796875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="15" t="s">
         <v>210</v>
       </c>
@@ -7432,7 +7432,7 @@
       </c>
       <c r="L1" s="16"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="15"/>
       <c r="B2" s="15"/>
       <c r="C2" s="15"/>
@@ -7444,7 +7444,7 @@
       <c r="K2" s="16"/>
       <c r="L2" s="16"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>190</v>
       </c>
@@ -7472,7 +7472,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>195</v>
       </c>
@@ -7502,7 +7502,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>195</v>
       </c>
@@ -7523,7 +7523,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>195</v>
       </c>
@@ -7544,7 +7544,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>195</v>
       </c>
@@ -7565,7 +7565,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>195</v>
       </c>
@@ -7586,7 +7586,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>195</v>
       </c>
@@ -7612,7 +7612,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>195</v>
       </c>
@@ -7635,7 +7635,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>195</v>
       </c>
@@ -7663,7 +7663,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>195</v>
       </c>
@@ -7680,7 +7680,7 @@
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>195</v>
       </c>
@@ -7697,7 +7697,7 @@
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>195</v>
       </c>
@@ -7714,7 +7714,7 @@
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>209</v>
       </c>
@@ -7724,16 +7724,14 @@
       <c r="C15" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>201</v>
-      </c>
+      <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>209</v>
       </c>
@@ -7750,7 +7748,7 @@
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>209</v>
       </c>
@@ -7767,7 +7765,7 @@
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>209</v>
       </c>
@@ -7791,7 +7789,7 @@
       <c r="K18" s="3"/>
       <c r="L18" s="3"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>209</v>
       </c>
@@ -7806,7 +7804,7 @@
       <c r="K19" s="3"/>
       <c r="L19" s="3"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>209</v>
       </c>
@@ -7821,7 +7819,7 @@
       <c r="K20" s="3"/>
       <c r="L20" s="3"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>209</v>
       </c>
@@ -7833,27 +7831,30 @@
       </c>
       <c r="D21" s="1" t="s">
         <v>201</v>
+      </c>
+      <c r="F21" t="s">
+        <v>206</v>
       </c>
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
       <c r="K21" s="3"/>
       <c r="L21" s="3"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
       <c r="C22" s="1"/>
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
       <c r="K22" s="3"/>
       <c r="L22" s="3"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
       <c r="C23" s="1"/>
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
       <c r="K23" s="3"/>
       <c r="L23" s="3"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="H24" s="3"/>
@@ -7861,422 +7862,422 @@
       <c r="K24" s="3"/>
       <c r="L24" s="3"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
       <c r="C25" s="1"/>
       <c r="H25" s="3"/>
       <c r="I25" s="3"/>
       <c r="K25" s="3"/>
       <c r="L25" s="3"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
       <c r="C26" s="1"/>
       <c r="H26" s="3"/>
       <c r="I26" s="3"/>
       <c r="K26" s="3"/>
       <c r="L26" s="3"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
       <c r="C27" s="1"/>
       <c r="H27" s="3"/>
       <c r="I27" s="3"/>
       <c r="K27" s="3"/>
       <c r="L27" s="3"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
       <c r="C28" s="1"/>
       <c r="H28" s="3"/>
       <c r="I28" s="3"/>
       <c r="K28" s="3"/>
       <c r="L28" s="3"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
       <c r="C29" s="1"/>
       <c r="H29" s="3"/>
       <c r="I29" s="3"/>
       <c r="K29" s="3"/>
       <c r="L29" s="3"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
       <c r="C30" s="1"/>
       <c r="H30" s="3"/>
       <c r="I30" s="3"/>
       <c r="K30" s="3"/>
       <c r="L30" s="3"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
       <c r="C31" s="1"/>
       <c r="H31" s="3"/>
       <c r="I31" s="3"/>
       <c r="K31" s="3"/>
       <c r="L31" s="3"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
       <c r="H32" s="3"/>
       <c r="I32" s="3"/>
       <c r="K32" s="3"/>
       <c r="L32" s="3"/>
     </row>
-    <row r="33" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="8:12" x14ac:dyDescent="0.35">
       <c r="H33" s="3"/>
       <c r="I33" s="3"/>
       <c r="K33" s="3"/>
       <c r="L33" s="3"/>
     </row>
-    <row r="34" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="8:12" x14ac:dyDescent="0.35">
       <c r="H34" s="3"/>
       <c r="I34" s="3"/>
       <c r="K34" s="3"/>
       <c r="L34" s="3"/>
     </row>
-    <row r="35" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="8:12" x14ac:dyDescent="0.35">
       <c r="H35" s="3"/>
       <c r="I35" s="3"/>
       <c r="K35" s="3"/>
       <c r="L35" s="3"/>
     </row>
-    <row r="36" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="8:12" x14ac:dyDescent="0.35">
       <c r="H36" s="3"/>
       <c r="I36" s="3"/>
       <c r="K36" s="3"/>
       <c r="L36" s="3"/>
     </row>
-    <row r="37" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="8:12" x14ac:dyDescent="0.35">
       <c r="H37" s="3"/>
       <c r="I37" s="3"/>
       <c r="K37" s="3"/>
       <c r="L37" s="3"/>
     </row>
-    <row r="38" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="8:12" x14ac:dyDescent="0.35">
       <c r="H38" s="3"/>
       <c r="I38" s="3"/>
       <c r="K38" s="3"/>
       <c r="L38" s="3"/>
     </row>
-    <row r="39" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="8:12" x14ac:dyDescent="0.35">
       <c r="H39" s="3"/>
       <c r="I39" s="3"/>
       <c r="K39" s="3"/>
       <c r="L39" s="3"/>
     </row>
-    <row r="40" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="8:12" x14ac:dyDescent="0.35">
       <c r="H40" s="3"/>
       <c r="I40" s="3"/>
       <c r="K40" s="3"/>
       <c r="L40" s="3"/>
     </row>
-    <row r="41" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="8:12" x14ac:dyDescent="0.35">
       <c r="H41" s="3"/>
       <c r="I41" s="3"/>
       <c r="K41" s="3"/>
       <c r="L41" s="3"/>
     </row>
-    <row r="42" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="8:12" x14ac:dyDescent="0.35">
       <c r="H42" s="3"/>
       <c r="I42" s="3"/>
       <c r="K42" s="3"/>
       <c r="L42" s="3"/>
     </row>
-    <row r="43" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="8:12" x14ac:dyDescent="0.35">
       <c r="H43" s="3"/>
       <c r="I43" s="3"/>
       <c r="K43" s="3"/>
       <c r="L43" s="3"/>
     </row>
-    <row r="44" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="8:12" x14ac:dyDescent="0.35">
       <c r="H44" s="3"/>
       <c r="I44" s="3"/>
       <c r="K44" s="3"/>
       <c r="L44" s="3"/>
     </row>
-    <row r="45" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="8:12" x14ac:dyDescent="0.35">
       <c r="H45" s="3"/>
       <c r="I45" s="3"/>
       <c r="K45" s="3"/>
       <c r="L45" s="3"/>
     </row>
-    <row r="46" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="8:12" x14ac:dyDescent="0.35">
       <c r="H46" s="3"/>
       <c r="I46" s="3"/>
       <c r="K46" s="3"/>
       <c r="L46" s="3"/>
     </row>
-    <row r="47" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="8:12" x14ac:dyDescent="0.35">
       <c r="H47" s="3"/>
       <c r="I47" s="3"/>
       <c r="K47" s="3"/>
       <c r="L47" s="3"/>
     </row>
-    <row r="48" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="8:12" x14ac:dyDescent="0.35">
       <c r="H48" s="3"/>
       <c r="I48" s="3"/>
       <c r="K48" s="3"/>
       <c r="L48" s="3"/>
     </row>
-    <row r="49" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="8:12" x14ac:dyDescent="0.35">
       <c r="H49" s="3"/>
       <c r="I49" s="3"/>
       <c r="K49" s="3"/>
       <c r="L49" s="3"/>
     </row>
-    <row r="50" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="8:12" x14ac:dyDescent="0.35">
       <c r="H50" s="3"/>
       <c r="I50" s="3"/>
       <c r="K50" s="3"/>
       <c r="L50" s="3"/>
     </row>
-    <row r="51" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="8:12" x14ac:dyDescent="0.35">
       <c r="H51" s="3"/>
       <c r="I51" s="3"/>
       <c r="K51" s="3"/>
       <c r="L51" s="3"/>
     </row>
-    <row r="52" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="8:12" x14ac:dyDescent="0.35">
       <c r="H52" s="3"/>
       <c r="I52" s="3"/>
       <c r="K52" s="3"/>
       <c r="L52" s="3"/>
     </row>
-    <row r="53" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="8:12" x14ac:dyDescent="0.35">
       <c r="H53" s="3"/>
       <c r="I53" s="3"/>
       <c r="K53" s="3"/>
       <c r="L53" s="3"/>
     </row>
-    <row r="54" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="8:12" x14ac:dyDescent="0.35">
       <c r="H54" s="3"/>
       <c r="I54" s="3"/>
       <c r="K54" s="3"/>
       <c r="L54" s="3"/>
     </row>
-    <row r="55" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="8:12" x14ac:dyDescent="0.35">
       <c r="H55" s="3"/>
       <c r="I55" s="3"/>
       <c r="K55" s="3"/>
       <c r="L55" s="3"/>
     </row>
-    <row r="56" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="8:12" x14ac:dyDescent="0.35">
       <c r="H56" s="3"/>
       <c r="I56" s="3"/>
       <c r="K56" s="3"/>
       <c r="L56" s="3"/>
     </row>
-    <row r="57" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="57" spans="8:12" x14ac:dyDescent="0.35">
       <c r="H57" s="3"/>
       <c r="I57" s="3"/>
       <c r="K57" s="3"/>
       <c r="L57" s="3"/>
     </row>
-    <row r="58" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="8:12" x14ac:dyDescent="0.35">
       <c r="H58" s="3"/>
       <c r="I58" s="3"/>
       <c r="K58" s="3"/>
       <c r="L58" s="3"/>
     </row>
-    <row r="59" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="59" spans="8:12" x14ac:dyDescent="0.35">
       <c r="H59" s="3"/>
       <c r="I59" s="3"/>
       <c r="K59" s="3"/>
       <c r="L59" s="3"/>
     </row>
-    <row r="60" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="60" spans="8:12" x14ac:dyDescent="0.35">
       <c r="H60" s="3"/>
       <c r="I60" s="3"/>
       <c r="K60" s="3"/>
       <c r="L60" s="3"/>
     </row>
-    <row r="61" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="61" spans="8:12" x14ac:dyDescent="0.35">
       <c r="H61" s="3"/>
       <c r="I61" s="3"/>
       <c r="K61" s="3"/>
       <c r="L61" s="3"/>
     </row>
-    <row r="62" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="62" spans="8:12" x14ac:dyDescent="0.35">
       <c r="H62" s="3"/>
       <c r="I62" s="3"/>
       <c r="K62" s="3"/>
       <c r="L62" s="3"/>
     </row>
-    <row r="63" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="63" spans="8:12" x14ac:dyDescent="0.35">
       <c r="H63" s="3"/>
       <c r="I63" s="3"/>
       <c r="K63" s="3"/>
       <c r="L63" s="3"/>
     </row>
-    <row r="64" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="64" spans="8:12" x14ac:dyDescent="0.35">
       <c r="H64" s="3"/>
       <c r="I64" s="3"/>
       <c r="K64" s="3"/>
       <c r="L64" s="3"/>
     </row>
-    <row r="65" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="65" spans="8:12" x14ac:dyDescent="0.35">
       <c r="H65" s="3"/>
       <c r="I65" s="3"/>
       <c r="K65" s="3"/>
       <c r="L65" s="3"/>
     </row>
-    <row r="66" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="66" spans="8:12" x14ac:dyDescent="0.35">
       <c r="H66" s="3"/>
       <c r="I66" s="3"/>
       <c r="K66" s="3"/>
       <c r="L66" s="3"/>
     </row>
-    <row r="67" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="67" spans="8:12" x14ac:dyDescent="0.35">
       <c r="H67" s="3"/>
       <c r="I67" s="3"/>
       <c r="K67" s="3"/>
       <c r="L67" s="3"/>
     </row>
-    <row r="68" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="68" spans="8:12" x14ac:dyDescent="0.35">
       <c r="H68" s="3"/>
       <c r="I68" s="3"/>
       <c r="K68" s="3"/>
       <c r="L68" s="3"/>
     </row>
-    <row r="69" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="69" spans="8:12" x14ac:dyDescent="0.35">
       <c r="H69" s="3"/>
       <c r="I69" s="3"/>
       <c r="K69" s="3"/>
       <c r="L69" s="3"/>
     </row>
-    <row r="70" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="70" spans="8:12" x14ac:dyDescent="0.35">
       <c r="H70" s="3"/>
       <c r="I70" s="3"/>
       <c r="K70" s="3"/>
       <c r="L70" s="3"/>
     </row>
-    <row r="71" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="71" spans="8:12" x14ac:dyDescent="0.35">
       <c r="H71" s="3"/>
       <c r="I71" s="3"/>
       <c r="K71" s="3"/>
       <c r="L71" s="3"/>
     </row>
-    <row r="72" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="72" spans="8:12" x14ac:dyDescent="0.35">
       <c r="H72" s="3"/>
       <c r="I72" s="3"/>
       <c r="K72" s="3"/>
       <c r="L72" s="3"/>
     </row>
-    <row r="73" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="73" spans="8:12" x14ac:dyDescent="0.35">
       <c r="H73" s="3"/>
       <c r="I73" s="3"/>
       <c r="K73" s="3"/>
       <c r="L73" s="3"/>
     </row>
-    <row r="74" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="74" spans="8:12" x14ac:dyDescent="0.35">
       <c r="H74" s="3"/>
       <c r="I74" s="3"/>
       <c r="K74" s="3"/>
       <c r="L74" s="3"/>
     </row>
-    <row r="75" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="75" spans="8:12" x14ac:dyDescent="0.35">
       <c r="H75" s="3"/>
       <c r="I75" s="3"/>
       <c r="K75" s="3"/>
       <c r="L75" s="3"/>
     </row>
-    <row r="76" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="76" spans="8:12" x14ac:dyDescent="0.35">
       <c r="H76" s="3"/>
       <c r="I76" s="3"/>
       <c r="K76" s="3"/>
       <c r="L76" s="3"/>
     </row>
-    <row r="77" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="77" spans="8:12" x14ac:dyDescent="0.35">
       <c r="H77" s="3"/>
       <c r="I77" s="3"/>
       <c r="K77" s="3"/>
       <c r="L77" s="3"/>
     </row>
-    <row r="78" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="78" spans="8:12" x14ac:dyDescent="0.35">
       <c r="H78" s="3"/>
       <c r="I78" s="3"/>
       <c r="K78" s="3"/>
       <c r="L78" s="3"/>
     </row>
-    <row r="79" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="79" spans="8:12" x14ac:dyDescent="0.35">
       <c r="H79" s="3"/>
       <c r="I79" s="3"/>
       <c r="K79" s="3"/>
       <c r="L79" s="3"/>
     </row>
-    <row r="80" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="80" spans="8:12" x14ac:dyDescent="0.35">
       <c r="H80" s="3"/>
       <c r="I80" s="3"/>
       <c r="K80" s="3"/>
       <c r="L80" s="3"/>
     </row>
-    <row r="81" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="81" spans="8:12" x14ac:dyDescent="0.35">
       <c r="H81" s="3"/>
       <c r="I81" s="3"/>
       <c r="K81" s="3"/>
       <c r="L81" s="3"/>
     </row>
-    <row r="82" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="82" spans="8:12" x14ac:dyDescent="0.35">
       <c r="H82" s="3"/>
       <c r="I82" s="3"/>
       <c r="K82" s="3"/>
       <c r="L82" s="3"/>
     </row>
-    <row r="83" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="83" spans="8:12" x14ac:dyDescent="0.35">
       <c r="H83" s="3"/>
       <c r="I83" s="3"/>
       <c r="K83" s="3"/>
       <c r="L83" s="3"/>
     </row>
-    <row r="84" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="84" spans="8:12" x14ac:dyDescent="0.35">
       <c r="H84" s="3"/>
       <c r="I84" s="3"/>
       <c r="K84" s="3"/>
       <c r="L84" s="3"/>
     </row>
-    <row r="85" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="85" spans="8:12" x14ac:dyDescent="0.35">
       <c r="H85" s="3"/>
       <c r="I85" s="3"/>
       <c r="K85" s="3"/>
       <c r="L85" s="3"/>
     </row>
-    <row r="86" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="86" spans="8:12" x14ac:dyDescent="0.35">
       <c r="H86" s="3"/>
       <c r="I86" s="3"/>
       <c r="K86" s="3"/>
       <c r="L86" s="3"/>
     </row>
-    <row r="87" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="87" spans="8:12" x14ac:dyDescent="0.35">
       <c r="H87" s="3"/>
       <c r="I87" s="3"/>
       <c r="K87" s="3"/>
       <c r="L87" s="3"/>
     </row>
-    <row r="88" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="88" spans="8:12" x14ac:dyDescent="0.35">
       <c r="H88" s="3"/>
       <c r="I88" s="3"/>
       <c r="K88" s="3"/>
       <c r="L88" s="3"/>
     </row>
-    <row r="89" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="89" spans="8:12" x14ac:dyDescent="0.35">
       <c r="H89" s="3"/>
       <c r="I89" s="3"/>
       <c r="K89" s="3"/>
       <c r="L89" s="3"/>
     </row>
-    <row r="90" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="90" spans="8:12" x14ac:dyDescent="0.35">
       <c r="H90" s="3"/>
       <c r="I90" s="3"/>
       <c r="K90" s="3"/>
       <c r="L90" s="3"/>
     </row>
-    <row r="91" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="91" spans="8:12" x14ac:dyDescent="0.35">
       <c r="H91" s="3"/>
       <c r="I91" s="3"/>
       <c r="K91" s="3"/>
       <c r="L91" s="3"/>
     </row>
-    <row r="92" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="92" spans="8:12" x14ac:dyDescent="0.35">
       <c r="H92" s="3"/>
       <c r="I92" s="3"/>
       <c r="K92" s="3"/>
       <c r="L92" s="3"/>
     </row>
-    <row r="93" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="93" spans="8:12" x14ac:dyDescent="0.35">
       <c r="H93" s="3"/>
       <c r="I93" s="3"/>
       <c r="K93" s="3"/>
@@ -8312,13 +8313,13 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" customWidth="1"/>
-    <col min="2" max="2" width="25.7109375" customWidth="1"/>
+    <col min="1" max="1" width="10.7265625" customWidth="1"/>
+    <col min="2" max="2" width="25.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="17" t="s">
         <v>220</v>
       </c>
@@ -8339,7 +8340,7 @@
       <c r="P1" s="8"/>
       <c r="Q1" s="10"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>219</v>
       </c>
@@ -8362,7 +8363,7 @@
       <c r="P2" s="11"/>
       <c r="Q2" s="10"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3" s="4"/>
       <c r="B3" s="5"/>
       <c r="C3" s="9"/>
@@ -8381,7 +8382,7 @@
       <c r="P3" s="11"/>
       <c r="Q3" s="10"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="C4" s="9"/>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -8398,7 +8399,7 @@
       <c r="P4" s="11"/>
       <c r="Q4" s="10"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="C5" s="9"/>
       <c r="D5" s="10"/>
       <c r="E5" s="10"/>
@@ -8415,7 +8416,7 @@
       <c r="P5" s="11"/>
       <c r="Q5" s="10"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="C6" s="9"/>
       <c r="D6" s="10"/>
       <c r="E6" s="10"/>
@@ -8432,7 +8433,7 @@
       <c r="P6" s="11"/>
       <c r="Q6" s="10"/>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="C7" s="9"/>
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
@@ -8449,7 +8450,7 @@
       <c r="P7" s="11"/>
       <c r="Q7" s="10"/>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="C8" s="9"/>
       <c r="D8" s="10"/>
       <c r="E8" s="10"/>
@@ -8466,7 +8467,7 @@
       <c r="P8" s="11"/>
       <c r="Q8" s="10"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="C9" s="9"/>
       <c r="D9" s="10"/>
       <c r="E9" s="10"/>
@@ -8483,7 +8484,7 @@
       <c r="P9" s="11"/>
       <c r="Q9" s="10"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="C10" s="9"/>
       <c r="D10" s="10"/>
       <c r="E10" s="10"/>
@@ -8500,7 +8501,7 @@
       <c r="P10" s="11"/>
       <c r="Q10" s="10"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="C11" s="9"/>
       <c r="D11" s="10"/>
       <c r="E11" s="10"/>
@@ -8517,7 +8518,7 @@
       <c r="P11" s="11"/>
       <c r="Q11" s="10"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="C12" s="9"/>
       <c r="D12" s="10"/>
       <c r="E12" s="10"/>
@@ -8534,7 +8535,7 @@
       <c r="P12" s="11"/>
       <c r="Q12" s="10"/>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="C13" s="9"/>
       <c r="D13" s="10"/>
       <c r="E13" s="10"/>
@@ -8551,7 +8552,7 @@
       <c r="P13" s="11"/>
       <c r="Q13" s="10"/>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="C14" s="9"/>
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
@@ -8568,7 +8569,7 @@
       <c r="P14" s="11"/>
       <c r="Q14" s="10"/>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="C15" s="9"/>
       <c r="D15" s="10"/>
       <c r="E15" s="10"/>
@@ -8585,7 +8586,7 @@
       <c r="P15" s="11"/>
       <c r="Q15" s="10"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="C16" s="9"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
@@ -8602,7 +8603,7 @@
       <c r="P16" s="11"/>
       <c r="Q16" s="10"/>
     </row>
-    <row r="17" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C17" s="9"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
@@ -8619,7 +8620,7 @@
       <c r="P17" s="11"/>
       <c r="Q17" s="10"/>
     </row>
-    <row r="18" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C18" s="9"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
@@ -8636,7 +8637,7 @@
       <c r="P18" s="11"/>
       <c r="Q18" s="10"/>
     </row>
-    <row r="19" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C19" s="9"/>
       <c r="D19" s="10"/>
       <c r="E19" s="10"/>
@@ -8653,7 +8654,7 @@
       <c r="P19" s="11"/>
       <c r="Q19" s="10"/>
     </row>
-    <row r="20" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C20" s="9"/>
       <c r="D20" s="10"/>
       <c r="E20" s="10"/>
@@ -8670,7 +8671,7 @@
       <c r="P20" s="11"/>
       <c r="Q20" s="10"/>
     </row>
-    <row r="21" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C21" s="9"/>
       <c r="D21" s="10"/>
       <c r="E21" s="10"/>
@@ -8687,7 +8688,7 @@
       <c r="P21" s="11"/>
       <c r="Q21" s="10"/>
     </row>
-    <row r="22" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C22" s="9"/>
       <c r="D22" s="10"/>
       <c r="E22" s="10"/>
@@ -8704,7 +8705,7 @@
       <c r="P22" s="11"/>
       <c r="Q22" s="10"/>
     </row>
-    <row r="23" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C23" s="9"/>
       <c r="D23" s="10"/>
       <c r="E23" s="10"/>
@@ -8721,7 +8722,7 @@
       <c r="P23" s="11"/>
       <c r="Q23" s="10"/>
     </row>
-    <row r="24" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C24" s="9"/>
       <c r="D24" s="10"/>
       <c r="E24" s="10"/>
@@ -8738,7 +8739,7 @@
       <c r="P24" s="11"/>
       <c r="Q24" s="10"/>
     </row>
-    <row r="25" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C25" s="9"/>
       <c r="D25" s="10"/>
       <c r="E25" s="10"/>
@@ -8755,7 +8756,7 @@
       <c r="P25" s="11"/>
       <c r="Q25" s="10"/>
     </row>
-    <row r="26" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C26" s="9"/>
       <c r="D26" s="10"/>
       <c r="E26" s="10"/>
@@ -8772,7 +8773,7 @@
       <c r="P26" s="11"/>
       <c r="Q26" s="10"/>
     </row>
-    <row r="27" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C27" s="9"/>
       <c r="D27" s="10"/>
       <c r="E27" s="10"/>
@@ -8789,7 +8790,7 @@
       <c r="P27" s="11"/>
       <c r="Q27" s="10"/>
     </row>
-    <row r="28" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C28" s="9"/>
       <c r="D28" s="10"/>
       <c r="E28" s="10"/>
@@ -8806,7 +8807,7 @@
       <c r="P28" s="11"/>
       <c r="Q28" s="10"/>
     </row>
-    <row r="29" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C29" s="9"/>
       <c r="D29" s="10"/>
       <c r="E29" s="10"/>
@@ -8823,7 +8824,7 @@
       <c r="P29" s="11"/>
       <c r="Q29" s="10"/>
     </row>
-    <row r="30" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="3:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C30" s="12"/>
       <c r="D30" s="13"/>
       <c r="E30" s="13"/>
@@ -8840,7 +8841,7 @@
       <c r="P30" s="14"/>
       <c r="Q30" s="10"/>
     </row>
-    <row r="31" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C31" s="10"/>
       <c r="D31" s="10"/>
       <c r="E31" s="10"/>
@@ -8873,13 +8874,13 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" customWidth="1"/>
-    <col min="2" max="2" width="25.7109375" customWidth="1"/>
+    <col min="1" max="1" width="10.7265625" customWidth="1"/>
+    <col min="2" max="2" width="25.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="17" t="s">
         <v>220</v>
       </c>
@@ -8899,7 +8900,7 @@
       <c r="O1" s="7"/>
       <c r="P1" s="8"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>219</v>
       </c>
@@ -8921,7 +8922,7 @@
       <c r="O2" s="10"/>
       <c r="P2" s="11"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3" s="4"/>
       <c r="B3" s="5"/>
       <c r="C3" s="9"/>
@@ -8939,7 +8940,7 @@
       <c r="O3" s="10"/>
       <c r="P3" s="11"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C4" s="9"/>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -8955,7 +8956,7 @@
       <c r="O4" s="10"/>
       <c r="P4" s="11"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C5" s="9"/>
       <c r="D5" s="10"/>
       <c r="E5" s="10"/>
@@ -8971,7 +8972,7 @@
       <c r="O5" s="10"/>
       <c r="P5" s="11"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C6" s="9"/>
       <c r="D6" s="10"/>
       <c r="E6" s="10"/>
@@ -8987,7 +8988,7 @@
       <c r="O6" s="10"/>
       <c r="P6" s="11"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C7" s="9"/>
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
@@ -9003,7 +9004,7 @@
       <c r="O7" s="10"/>
       <c r="P7" s="11"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C8" s="9"/>
       <c r="D8" s="10"/>
       <c r="E8" s="10"/>
@@ -9019,7 +9020,7 @@
       <c r="O8" s="10"/>
       <c r="P8" s="11"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C9" s="9"/>
       <c r="D9" s="10"/>
       <c r="E9" s="10"/>
@@ -9035,7 +9036,7 @@
       <c r="O9" s="10"/>
       <c r="P9" s="11"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C10" s="9"/>
       <c r="D10" s="10"/>
       <c r="E10" s="10"/>
@@ -9051,7 +9052,7 @@
       <c r="O10" s="10"/>
       <c r="P10" s="11"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C11" s="9"/>
       <c r="D11" s="10"/>
       <c r="E11" s="10"/>
@@ -9067,7 +9068,7 @@
       <c r="O11" s="10"/>
       <c r="P11" s="11"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C12" s="9"/>
       <c r="D12" s="10"/>
       <c r="E12" s="10"/>
@@ -9083,7 +9084,7 @@
       <c r="O12" s="10"/>
       <c r="P12" s="11"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C13" s="9"/>
       <c r="D13" s="10"/>
       <c r="E13" s="10"/>
@@ -9099,7 +9100,7 @@
       <c r="O13" s="10"/>
       <c r="P13" s="11"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C14" s="9"/>
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
@@ -9115,7 +9116,7 @@
       <c r="O14" s="10"/>
       <c r="P14" s="11"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C15" s="9"/>
       <c r="D15" s="10"/>
       <c r="E15" s="10"/>
@@ -9131,7 +9132,7 @@
       <c r="O15" s="10"/>
       <c r="P15" s="11"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C16" s="9"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
@@ -9147,7 +9148,7 @@
       <c r="O16" s="10"/>
       <c r="P16" s="11"/>
     </row>
-    <row r="17" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C17" s="9"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
@@ -9163,7 +9164,7 @@
       <c r="O17" s="10"/>
       <c r="P17" s="11"/>
     </row>
-    <row r="18" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C18" s="9"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
@@ -9179,7 +9180,7 @@
       <c r="O18" s="10"/>
       <c r="P18" s="11"/>
     </row>
-    <row r="19" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C19" s="9"/>
       <c r="D19" s="10"/>
       <c r="E19" s="10"/>
@@ -9195,7 +9196,7 @@
       <c r="O19" s="10"/>
       <c r="P19" s="11"/>
     </row>
-    <row r="20" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C20" s="9"/>
       <c r="D20" s="10"/>
       <c r="E20" s="10"/>
@@ -9211,7 +9212,7 @@
       <c r="O20" s="10"/>
       <c r="P20" s="11"/>
     </row>
-    <row r="21" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C21" s="9"/>
       <c r="D21" s="10"/>
       <c r="E21" s="10"/>
@@ -9227,7 +9228,7 @@
       <c r="O21" s="10"/>
       <c r="P21" s="11"/>
     </row>
-    <row r="22" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C22" s="9"/>
       <c r="D22" s="10"/>
       <c r="E22" s="10"/>
@@ -9243,7 +9244,7 @@
       <c r="O22" s="10"/>
       <c r="P22" s="11"/>
     </row>
-    <row r="23" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C23" s="9"/>
       <c r="D23" s="10"/>
       <c r="E23" s="10"/>
@@ -9259,7 +9260,7 @@
       <c r="O23" s="10"/>
       <c r="P23" s="11"/>
     </row>
-    <row r="24" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C24" s="9"/>
       <c r="D24" s="10"/>
       <c r="E24" s="10"/>
@@ -9275,7 +9276,7 @@
       <c r="O24" s="10"/>
       <c r="P24" s="11"/>
     </row>
-    <row r="25" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C25" s="9"/>
       <c r="D25" s="10"/>
       <c r="E25" s="10"/>
@@ -9291,7 +9292,7 @@
       <c r="O25" s="10"/>
       <c r="P25" s="11"/>
     </row>
-    <row r="26" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C26" s="9"/>
       <c r="D26" s="10"/>
       <c r="E26" s="10"/>
@@ -9307,7 +9308,7 @@
       <c r="O26" s="10"/>
       <c r="P26" s="11"/>
     </row>
-    <row r="27" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C27" s="9"/>
       <c r="D27" s="10"/>
       <c r="E27" s="10"/>
@@ -9323,7 +9324,7 @@
       <c r="O27" s="10"/>
       <c r="P27" s="11"/>
     </row>
-    <row r="28" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C28" s="9"/>
       <c r="D28" s="10"/>
       <c r="E28" s="10"/>
@@ -9339,7 +9340,7 @@
       <c r="O28" s="10"/>
       <c r="P28" s="11"/>
     </row>
-    <row r="29" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C29" s="9"/>
       <c r="D29" s="10"/>
       <c r="E29" s="10"/>
@@ -9355,7 +9356,7 @@
       <c r="O29" s="10"/>
       <c r="P29" s="11"/>
     </row>
-    <row r="30" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="3:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C30" s="12"/>
       <c r="D30" s="13"/>
       <c r="E30" s="13"/>
@@ -9387,13 +9388,13 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" customWidth="1"/>
-    <col min="2" max="2" width="25.7109375" customWidth="1"/>
+    <col min="1" max="1" width="10.7265625" customWidth="1"/>
+    <col min="2" max="2" width="25.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="17" t="s">
         <v>220</v>
       </c>
@@ -9413,7 +9414,7 @@
       <c r="O1" s="7"/>
       <c r="P1" s="8"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>219</v>
       </c>
@@ -9435,7 +9436,7 @@
       <c r="O2" s="10"/>
       <c r="P2" s="11"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3" s="4"/>
       <c r="B3" s="5"/>
       <c r="C3" s="9"/>
@@ -9453,7 +9454,7 @@
       <c r="O3" s="10"/>
       <c r="P3" s="11"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C4" s="9"/>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -9469,7 +9470,7 @@
       <c r="O4" s="10"/>
       <c r="P4" s="11"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C5" s="9"/>
       <c r="D5" s="10"/>
       <c r="E5" s="10"/>
@@ -9485,7 +9486,7 @@
       <c r="O5" s="10"/>
       <c r="P5" s="11"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C6" s="9"/>
       <c r="D6" s="10"/>
       <c r="E6" s="10"/>
@@ -9501,7 +9502,7 @@
       <c r="O6" s="10"/>
       <c r="P6" s="11"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C7" s="9"/>
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
@@ -9517,7 +9518,7 @@
       <c r="O7" s="10"/>
       <c r="P7" s="11"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C8" s="9"/>
       <c r="D8" s="10"/>
       <c r="E8" s="10"/>
@@ -9533,7 +9534,7 @@
       <c r="O8" s="10"/>
       <c r="P8" s="11"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C9" s="9"/>
       <c r="D9" s="10"/>
       <c r="E9" s="10"/>
@@ -9549,7 +9550,7 @@
       <c r="O9" s="10"/>
       <c r="P9" s="11"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C10" s="9"/>
       <c r="D10" s="10"/>
       <c r="E10" s="10"/>
@@ -9565,7 +9566,7 @@
       <c r="O10" s="10"/>
       <c r="P10" s="11"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C11" s="9"/>
       <c r="D11" s="10"/>
       <c r="E11" s="10"/>
@@ -9581,7 +9582,7 @@
       <c r="O11" s="10"/>
       <c r="P11" s="11"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C12" s="9"/>
       <c r="D12" s="10"/>
       <c r="E12" s="10"/>
@@ -9597,7 +9598,7 @@
       <c r="O12" s="10"/>
       <c r="P12" s="11"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C13" s="9"/>
       <c r="D13" s="10"/>
       <c r="E13" s="10"/>
@@ -9613,7 +9614,7 @@
       <c r="O13" s="10"/>
       <c r="P13" s="11"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C14" s="9"/>
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
@@ -9629,7 +9630,7 @@
       <c r="O14" s="10"/>
       <c r="P14" s="11"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C15" s="9"/>
       <c r="D15" s="10"/>
       <c r="E15" s="10"/>
@@ -9645,7 +9646,7 @@
       <c r="O15" s="10"/>
       <c r="P15" s="11"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C16" s="9"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
@@ -9661,7 +9662,7 @@
       <c r="O16" s="10"/>
       <c r="P16" s="11"/>
     </row>
-    <row r="17" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C17" s="9"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
@@ -9677,7 +9678,7 @@
       <c r="O17" s="10"/>
       <c r="P17" s="11"/>
     </row>
-    <row r="18" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C18" s="9"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
@@ -9693,7 +9694,7 @@
       <c r="O18" s="10"/>
       <c r="P18" s="11"/>
     </row>
-    <row r="19" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C19" s="9"/>
       <c r="D19" s="10"/>
       <c r="E19" s="10"/>
@@ -9709,7 +9710,7 @@
       <c r="O19" s="10"/>
       <c r="P19" s="11"/>
     </row>
-    <row r="20" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C20" s="9"/>
       <c r="D20" s="10"/>
       <c r="E20" s="10"/>
@@ -9725,7 +9726,7 @@
       <c r="O20" s="10"/>
       <c r="P20" s="11"/>
     </row>
-    <row r="21" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C21" s="9"/>
       <c r="D21" s="10"/>
       <c r="E21" s="10"/>
@@ -9741,7 +9742,7 @@
       <c r="O21" s="10"/>
       <c r="P21" s="11"/>
     </row>
-    <row r="22" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C22" s="9"/>
       <c r="D22" s="10"/>
       <c r="E22" s="10"/>
@@ -9757,7 +9758,7 @@
       <c r="O22" s="10"/>
       <c r="P22" s="11"/>
     </row>
-    <row r="23" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C23" s="9"/>
       <c r="D23" s="10"/>
       <c r="E23" s="10"/>
@@ -9773,7 +9774,7 @@
       <c r="O23" s="10"/>
       <c r="P23" s="11"/>
     </row>
-    <row r="24" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C24" s="9"/>
       <c r="D24" s="10"/>
       <c r="E24" s="10"/>
@@ -9789,7 +9790,7 @@
       <c r="O24" s="10"/>
       <c r="P24" s="11"/>
     </row>
-    <row r="25" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C25" s="9"/>
       <c r="D25" s="10"/>
       <c r="E25" s="10"/>
@@ -9805,7 +9806,7 @@
       <c r="O25" s="10"/>
       <c r="P25" s="11"/>
     </row>
-    <row r="26" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C26" s="9"/>
       <c r="D26" s="10"/>
       <c r="E26" s="10"/>
@@ -9821,7 +9822,7 @@
       <c r="O26" s="10"/>
       <c r="P26" s="11"/>
     </row>
-    <row r="27" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C27" s="9"/>
       <c r="D27" s="10"/>
       <c r="E27" s="10"/>
@@ -9837,7 +9838,7 @@
       <c r="O27" s="10"/>
       <c r="P27" s="11"/>
     </row>
-    <row r="28" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C28" s="9"/>
       <c r="D28" s="10"/>
       <c r="E28" s="10"/>
@@ -9853,7 +9854,7 @@
       <c r="O28" s="10"/>
       <c r="P28" s="11"/>
     </row>
-    <row r="29" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C29" s="9"/>
       <c r="D29" s="10"/>
       <c r="E29" s="10"/>
@@ -9869,7 +9870,7 @@
       <c r="O29" s="10"/>
       <c r="P29" s="11"/>
     </row>
-    <row r="30" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="3:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C30" s="12"/>
       <c r="D30" s="13"/>
       <c r="E30" s="13"/>
@@ -9901,13 +9902,13 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" customWidth="1"/>
-    <col min="2" max="2" width="25.7109375" customWidth="1"/>
+    <col min="1" max="1" width="10.7265625" customWidth="1"/>
+    <col min="2" max="2" width="25.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="17" t="s">
         <v>220</v>
       </c>
@@ -9927,7 +9928,7 @@
       <c r="O1" s="7"/>
       <c r="P1" s="8"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>219</v>
       </c>
@@ -9949,7 +9950,7 @@
       <c r="O2" s="10"/>
       <c r="P2" s="11"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3" s="4"/>
       <c r="B3" s="5"/>
       <c r="C3" s="9"/>
@@ -9967,7 +9968,7 @@
       <c r="O3" s="10"/>
       <c r="P3" s="11"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C4" s="9"/>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -9983,7 +9984,7 @@
       <c r="O4" s="10"/>
       <c r="P4" s="11"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C5" s="9"/>
       <c r="D5" s="10"/>
       <c r="E5" s="10"/>
@@ -9999,7 +10000,7 @@
       <c r="O5" s="10"/>
       <c r="P5" s="11"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C6" s="9"/>
       <c r="D6" s="10"/>
       <c r="E6" s="10"/>
@@ -10015,7 +10016,7 @@
       <c r="O6" s="10"/>
       <c r="P6" s="11"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C7" s="9"/>
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
@@ -10031,7 +10032,7 @@
       <c r="O7" s="10"/>
       <c r="P7" s="11"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C8" s="9"/>
       <c r="D8" s="10"/>
       <c r="E8" s="10"/>
@@ -10047,7 +10048,7 @@
       <c r="O8" s="10"/>
       <c r="P8" s="11"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C9" s="9"/>
       <c r="D9" s="10"/>
       <c r="E9" s="10"/>
@@ -10063,7 +10064,7 @@
       <c r="O9" s="10"/>
       <c r="P9" s="11"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C10" s="9"/>
       <c r="D10" s="10"/>
       <c r="E10" s="10"/>
@@ -10079,7 +10080,7 @@
       <c r="O10" s="10"/>
       <c r="P10" s="11"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C11" s="9"/>
       <c r="D11" s="10"/>
       <c r="E11" s="10"/>
@@ -10095,7 +10096,7 @@
       <c r="O11" s="10"/>
       <c r="P11" s="11"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C12" s="9"/>
       <c r="D12" s="10"/>
       <c r="E12" s="10"/>
@@ -10111,7 +10112,7 @@
       <c r="O12" s="10"/>
       <c r="P12" s="11"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C13" s="9"/>
       <c r="D13" s="10"/>
       <c r="E13" s="10"/>
@@ -10127,7 +10128,7 @@
       <c r="O13" s="10"/>
       <c r="P13" s="11"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C14" s="9"/>
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
@@ -10143,7 +10144,7 @@
       <c r="O14" s="10"/>
       <c r="P14" s="11"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C15" s="9"/>
       <c r="D15" s="10"/>
       <c r="E15" s="10"/>
@@ -10159,7 +10160,7 @@
       <c r="O15" s="10"/>
       <c r="P15" s="11"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C16" s="9"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
@@ -10175,7 +10176,7 @@
       <c r="O16" s="10"/>
       <c r="P16" s="11"/>
     </row>
-    <row r="17" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C17" s="9"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
@@ -10191,7 +10192,7 @@
       <c r="O17" s="10"/>
       <c r="P17" s="11"/>
     </row>
-    <row r="18" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C18" s="9"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
@@ -10207,7 +10208,7 @@
       <c r="O18" s="10"/>
       <c r="P18" s="11"/>
     </row>
-    <row r="19" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C19" s="9"/>
       <c r="D19" s="10"/>
       <c r="E19" s="10"/>
@@ -10223,7 +10224,7 @@
       <c r="O19" s="10"/>
       <c r="P19" s="11"/>
     </row>
-    <row r="20" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C20" s="9"/>
       <c r="D20" s="10"/>
       <c r="E20" s="10"/>
@@ -10239,7 +10240,7 @@
       <c r="O20" s="10"/>
       <c r="P20" s="11"/>
     </row>
-    <row r="21" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C21" s="9"/>
       <c r="D21" s="10"/>
       <c r="E21" s="10"/>
@@ -10255,7 +10256,7 @@
       <c r="O21" s="10"/>
       <c r="P21" s="11"/>
     </row>
-    <row r="22" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C22" s="9"/>
       <c r="D22" s="10"/>
       <c r="E22" s="10"/>
@@ -10271,7 +10272,7 @@
       <c r="O22" s="10"/>
       <c r="P22" s="11"/>
     </row>
-    <row r="23" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C23" s="9"/>
       <c r="D23" s="10"/>
       <c r="E23" s="10"/>
@@ -10287,7 +10288,7 @@
       <c r="O23" s="10"/>
       <c r="P23" s="11"/>
     </row>
-    <row r="24" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C24" s="9"/>
       <c r="D24" s="10"/>
       <c r="E24" s="10"/>
@@ -10303,7 +10304,7 @@
       <c r="O24" s="10"/>
       <c r="P24" s="11"/>
     </row>
-    <row r="25" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C25" s="9"/>
       <c r="D25" s="10"/>
       <c r="E25" s="10"/>
@@ -10319,7 +10320,7 @@
       <c r="O25" s="10"/>
       <c r="P25" s="11"/>
     </row>
-    <row r="26" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C26" s="9"/>
       <c r="D26" s="10"/>
       <c r="E26" s="10"/>
@@ -10335,7 +10336,7 @@
       <c r="O26" s="10"/>
       <c r="P26" s="11"/>
     </row>
-    <row r="27" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C27" s="9"/>
       <c r="D27" s="10"/>
       <c r="E27" s="10"/>
@@ -10351,7 +10352,7 @@
       <c r="O27" s="10"/>
       <c r="P27" s="11"/>
     </row>
-    <row r="28" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C28" s="9"/>
       <c r="D28" s="10"/>
       <c r="E28" s="10"/>
@@ -10367,7 +10368,7 @@
       <c r="O28" s="10"/>
       <c r="P28" s="11"/>
     </row>
-    <row r="29" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C29" s="9"/>
       <c r="D29" s="10"/>
       <c r="E29" s="10"/>
@@ -10383,7 +10384,7 @@
       <c r="O29" s="10"/>
       <c r="P29" s="11"/>
     </row>
-    <row r="30" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="3:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C30" s="12"/>
       <c r="D30" s="13"/>
       <c r="E30" s="13"/>

</xml_diff>